<commit_message>
correzzioni email support Accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maybesrloffice-my.sharepoint.com/personal/c_granata_inquery_it/Documents/Documenti/AccreditamentoFSE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84B4039E-25D7-451C-A2D8-AC0AF45E706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72CD227-D5C1-4B16-8B23-8BD648AEB7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="191">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -801,9 +801,6 @@
   </si>
   <si>
     <t>Non vienono gestite le allergie</t>
-  </si>
-  <si>
-    <t>Elenco preimpostato</t>
   </si>
   <si>
     <t>2024-11-26T12:01:43Z</t>
@@ -3109,10 +3106,10 @@
   <dimension ref="A1:W632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3185,7 +3182,7 @@
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="61"/>
       <c r="F3" s="6"/>
@@ -3211,7 +3208,7 @@
       <c r="A4" s="65"/>
       <c r="B4" s="66"/>
       <c r="C4" s="69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="4"/>
@@ -3238,7 +3235,7 @@
       <c r="A5" s="67"/>
       <c r="B5" s="68"/>
       <c r="C5" s="69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D5" s="61"/>
       <c r="F5" s="6"/>
@@ -4492,9 +4489,15 @@
       <c r="M37" s="34"/>
       <c r="N37" s="34"/>
       <c r="O37" s="34"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="34"/>
+      <c r="P37" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q37" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R37" s="34" t="s">
+        <v>101</v>
+      </c>
       <c r="S37" s="34" t="s">
         <v>177</v>
       </c>
@@ -4746,9 +4749,7 @@
       <c r="K43" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="L43" s="34" t="s">
-        <v>182</v>
-      </c>
+      <c r="L43" s="34"/>
       <c r="M43" s="34"/>
       <c r="N43" s="34"/>
       <c r="O43" s="34"/>
@@ -4874,13 +4875,13 @@
         <v>45622</v>
       </c>
       <c r="G47" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="H47" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="H47" s="42" t="s">
+      <c r="I47" s="42" t="s">
         <v>184</v>
-      </c>
-      <c r="I47" s="42" t="s">
-        <v>185</v>
       </c>
       <c r="J47" s="43" t="s">
         <v>51</v>
@@ -4921,13 +4922,13 @@
         <v>45622</v>
       </c>
       <c r="G48" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="H48" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="H48" s="49" t="s">
+      <c r="I48" s="49" t="s">
         <v>187</v>
-      </c>
-      <c r="I48" s="49" t="s">
-        <v>188</v>
       </c>
       <c r="J48" s="50" t="s">
         <v>51</v>
@@ -11826,6 +11827,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12083,42 +12105,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12141,9 +12131,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
campo  con valori specifici
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72CD227-D5C1-4B16-8B23-8BD648AEB7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A39ECD-DA4A-4497-823B-1FF44BD71299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="191">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3106,10 +3106,10 @@
   <dimension ref="A1:W632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
+      <selection pane="bottomRight" activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4484,7 +4484,9 @@
       <c r="J37" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K37" s="34"/>
+      <c r="K37" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L37" s="34"/>
       <c r="M37" s="34"/>
       <c r="N37" s="34"/>
@@ -11827,27 +11829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12105,10 +12086,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12131,20 +12144,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cambio file con CDA obbligatori per l'accreditamento
cambio file con CDA obbligatori per l'accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A39ECD-DA4A-4497-823B-1FF44BD71299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B264B2DE-DB44-4DD8-960C-0971E27D3382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,21 +803,6 @@
     <t>Non vienono gestite le allergie</t>
   </si>
   <si>
-    <t>2024-11-26T12:01:43Z</t>
-  </si>
-  <si>
-    <t>dbc1da5b87a28759</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.89228d803b78f561135a6b020a018ca8fd64aacd77a1c3d66f972b0ac562511c.4d069d01a6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-11-26T12:07:48Z</t>
-  </si>
-  <si>
-    <t>d424d34ddc07d91d</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.89228d803b78f561135a6b020a018ca8fd64aacd77a1c3d66f972b0ac562511c.b44e63838a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -828,6 +813,21 @@
   </si>
   <si>
     <t>subject_application_version:1.0.0.0</t>
+  </si>
+  <si>
+    <t>9fc098b652b75a5c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a0fd93e64bbe3838610303f81f165e84adbf52a1e7f61fa016e79db5e28c5b6f.e26d4334dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-12-18T12:05:48Z</t>
+  </si>
+  <si>
+    <t>196c8dbfd9400665</t>
+  </si>
+  <si>
+    <t>2024-12-18T11:55:43Z</t>
   </si>
 </sst>
 </file>
@@ -3106,10 +3106,10 @@
   <dimension ref="A1:W632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L37" sqref="L37"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="69" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D3" s="61"/>
       <c r="F3" s="6"/>
@@ -3208,7 +3208,7 @@
       <c r="A4" s="65"/>
       <c r="B4" s="66"/>
       <c r="C4" s="69" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="4"/>
@@ -3235,7 +3235,7 @@
       <c r="A5" s="67"/>
       <c r="B5" s="68"/>
       <c r="C5" s="69" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D5" s="61"/>
       <c r="F5" s="6"/>
@@ -4874,16 +4874,16 @@
         <v>127</v>
       </c>
       <c r="F47" s="41">
-        <v>45622</v>
+        <v>45644</v>
       </c>
       <c r="G47" s="42" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="H47" s="42" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="I47" s="42" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J47" s="43" t="s">
         <v>51</v>
@@ -4921,16 +4921,16 @@
         <v>128</v>
       </c>
       <c r="F48" s="48">
-        <v>45622</v>
+        <v>45644</v>
       </c>
       <c r="G48" s="49" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H48" s="49" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I48" s="49" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="J48" s="50" t="s">
         <v>51</v>
@@ -11829,6 +11829,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12086,42 +12107,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12144,9 +12133,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cda rad con campi obbligatori
cda rad con campi obbligatori
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A39ECD-DA4A-4497-823B-1FF44BD71299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B264B2DE-DB44-4DD8-960C-0971E27D3382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,21 +803,6 @@
     <t>Non vienono gestite le allergie</t>
   </si>
   <si>
-    <t>2024-11-26T12:01:43Z</t>
-  </si>
-  <si>
-    <t>dbc1da5b87a28759</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.89228d803b78f561135a6b020a018ca8fd64aacd77a1c3d66f972b0ac562511c.4d069d01a6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-11-26T12:07:48Z</t>
-  </si>
-  <si>
-    <t>d424d34ddc07d91d</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.89228d803b78f561135a6b020a018ca8fd64aacd77a1c3d66f972b0ac562511c.b44e63838a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -828,6 +813,21 @@
   </si>
   <si>
     <t>subject_application_version:1.0.0.0</t>
+  </si>
+  <si>
+    <t>9fc098b652b75a5c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a0fd93e64bbe3838610303f81f165e84adbf52a1e7f61fa016e79db5e28c5b6f.e26d4334dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-12-18T12:05:48Z</t>
+  </si>
+  <si>
+    <t>196c8dbfd9400665</t>
+  </si>
+  <si>
+    <t>2024-12-18T11:55:43Z</t>
   </si>
 </sst>
 </file>
@@ -3106,10 +3106,10 @@
   <dimension ref="A1:W632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L37" sqref="L37"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="69" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D3" s="61"/>
       <c r="F3" s="6"/>
@@ -3208,7 +3208,7 @@
       <c r="A4" s="65"/>
       <c r="B4" s="66"/>
       <c r="C4" s="69" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="4"/>
@@ -3235,7 +3235,7 @@
       <c r="A5" s="67"/>
       <c r="B5" s="68"/>
       <c r="C5" s="69" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D5" s="61"/>
       <c r="F5" s="6"/>
@@ -4874,16 +4874,16 @@
         <v>127</v>
       </c>
       <c r="F47" s="41">
-        <v>45622</v>
+        <v>45644</v>
       </c>
       <c r="G47" s="42" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="H47" s="42" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="I47" s="42" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J47" s="43" t="s">
         <v>51</v>
@@ -4921,16 +4921,16 @@
         <v>128</v>
       </c>
       <c r="F48" s="48">
-        <v>45622</v>
+        <v>45644</v>
       </c>
       <c r="G48" s="49" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H48" s="49" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I48" s="49" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="J48" s="50" t="s">
         <v>51</v>
@@ -11829,6 +11829,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12086,42 +12107,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12144,9 +12133,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix  bug suggerimento medico
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A069D21A-3D24-4DC9-B2EC-45EE3BAD717D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76930517-3941-41AA-BC81-025ADBF1F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,22 +812,22 @@
     <t>2025-01-22T11:48:27Z</t>
   </si>
   <si>
-    <t>2025-01-22T12:02:09Z</t>
-  </si>
-  <si>
-    <t>971a6c5cd634bf61</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.751fd78948^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f5c579880d6890a5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ac0bb01630^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-01-22T12:27:27Z</t>
+    <t>2025-01-28T17:12:22Z</t>
+  </si>
+  <si>
+    <t>f50dcb10bc026fb6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.3d68c8102e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-01-28T17:07:33Z</t>
+  </si>
+  <si>
+    <t>8c00ca714c870ae9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.d63c6b2c88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3109,7 +3109,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4874,7 +4874,7 @@
         <v>127</v>
       </c>
       <c r="F47" s="41">
-        <v>45677</v>
+        <v>45685</v>
       </c>
       <c r="G47" s="42" t="s">
         <v>185</v>
@@ -4921,16 +4921,16 @@
         <v>128</v>
       </c>
       <c r="F48" s="48">
-        <v>45677</v>
+        <v>45685</v>
       </c>
       <c r="G48" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="H48" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="I48" s="49" t="s">
         <v>190</v>
-      </c>
-      <c r="H48" s="49" t="s">
-        <v>188</v>
-      </c>
-      <c r="I48" s="49" t="s">
-        <v>189</v>
       </c>
       <c r="J48" s="50" t="s">
         <v>51</v>
@@ -11829,6 +11829,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12086,42 +12107,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12144,9 +12133,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix file json xls
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76930517-3941-41AA-BC81-025ADBF1F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D08A02-5178-4706-A687-C51D443A26DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$60</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="325">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -828,6 +828,437 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.d63c6b2c88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2025-02-02T18:45:59Z</t>
+  </si>
+  <si>
+    <t>4e7664ac1c33c161</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.cb0f4e1eb9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2025-02-03T16:58:24Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.6c550f02e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8555dbcac8c5751b</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2025-02-03T17:35:26Z</t>
+  </si>
+  <si>
+    <t>4adf0eb3a689a290</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.562d3ce0fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2025-02-04T12:41:28Z</t>
+  </si>
+  <si>
+    <t>2f6f11739b90d6e8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.60ce93b68e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2025-01-03T14:28:58Z</t>
+  </si>
+  <si>
+    <t>f0abc2dec788a4c3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.e18d2ba9e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore di sintassi: ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
+  </si>
+  <si>
+    <t>L'errore viene gestito a livello di applicazione alla produzione del referto</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>L'errore viene gestito dall'applicaizone con il controllo del codice fiscale</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT7_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>Prima di effettuare l'invio viene validato il file e controllato</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.23195b441f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.cc9a571001^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il controllo del file xml viene eseguito prima dell'invio</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>c4adc4670c76ce65</t>
+  </si>
+  <si>
+    <t>Errore gestito dallìapplicaizone, controllando prima la valiazione</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>[ERRORE-b4| Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento 'text'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>Non è possibile inviare se la sezione è vuota, controllo dell'applicazione</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>Controllo dei campi obbligaotri e verifica prima dell'invio</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene gestito l'obbligatorietà dei valori</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>l campo effectivetime/low ha sempre un valore di default, se non è presente la data perché non è disponbile (es. il paziente non ricorda) allora è presente il valore @nullFlavor = “UNK”.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>62d028544054dd72</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.a2aef11856^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-b36| Sezione Storia Clinica: l'elemento entry/organizer/subject/relatedSubject deve avere l'attributo @classCode='PRS' e deve contenere l'elemento 'code'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>Gestito dall'aplicaizone</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Gestito dall'applicazione campo obbligatorio</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>"Errore semantico. [ERRORE-44| Il codice fiscale '0012132145' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]"</t>
+  </si>
+  <si>
+    <t>a83bd16efcf9de0d</t>
+  </si>
+  <si>
+    <t>workflowInstanceId":"2.16.840.1.113883.2.9.2.120.4.4.758ddd9e38865de2ce747bb084caaf34b3f04d250edf0f79b491b5322fe0862f.930b68af3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T15:30:08Z</t>
+  </si>
+  <si>
+    <t>b2346e487feac030</t>
+  </si>
+  <si>
+    <t>2025-02-04T15:36:52Z</t>
+  </si>
+  <si>
+    <t>da883b8cd9c0542e</t>
+  </si>
+  <si>
+    <t>2025-02-04T16:33:05Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.c04afd54de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore di sintassi. ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'priorityCode'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected</t>
+  </si>
+  <si>
+    <t>2025-02-04T16:58:36Z</t>
+  </si>
+  <si>
+    <t>860af4e087971bb6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.6b9df4a85d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.,ERROR: -1,-1 cvc-datatype-valid.1.2.3: '' is not a valid value of union type 'uid'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'codeSystem' on element 'code' is not valid with respect to its type, 'uid'."</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:09:57Z</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:15:09Z</t>
+  </si>
+  <si>
+    <t>e34b8cb72eda5b7d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ccc318dc89^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:21:17Z</t>
+  </si>
+  <si>
+    <t>6cb600782a006772</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.59c944599d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:36:02Z</t>
+  </si>
+  <si>
+    <t>8e55629de097fdb4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.4a9ca2fe7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:51:45Z</t>
+  </si>
+  <si>
+    <t>"[ERRORE-b53| Sotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]"</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:55:47Z</t>
+  </si>
+  <si>
+    <t>b159f3ef01bdef63</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.0a2f34d7b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
+  </si>
+  <si>
+    <t>2025-01-03T12:48:01Z</t>
+  </si>
+  <si>
+    <t>8c22d910bd845ebc</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di token non valido all'utente</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
+  </si>
+  <si>
+    <t>2025-01-03T13:07:58Z</t>
+  </si>
+  <si>
+    <t>5461d8a35b4a54f7</t>
+  </si>
+  <si>
+    <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
+  </si>
+  <si>
+    <t>Viene fornito un messaggio di errore all'utente, campi token non validi</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_RSA_TIMEOUT</t>
+  </si>
+  <si>
+    <t>timeout servizio FSE</t>
+  </si>
+  <si>
+    <t>2025-02-12T13:44:10Z</t>
+  </si>
+  <si>
+    <t>667b3f100bd7d00b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ca19dd635e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-b21| Sezione Quesito Diagnostico: l'elemento entry/observation/code deve avere l'attributo @code='29298-7' e l'attributo @codeSystem='2.16.840.1.113883.6.1'],[ERRORE-b53| Sotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
+  </si>
+  <si>
+    <t>2025-02-12T13:49:51Z</t>
+  </si>
+  <si>
+    <t>2025-02-12T14:28:16Z</t>
+  </si>
+  <si>
+    <t>e9124089694e6dcb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ffcc1560c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1957,7 +2388,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3103,13 +3534,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:W632"/>
+  <dimension ref="A1:W620"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
+      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3394,218 +3825,522 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
+    <row r="10" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>31</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="32">
+        <v>45679</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
+      <c r="M10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="P10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R10" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>143</v>
+      </c>
       <c r="T10" s="34"/>
-      <c r="U10" s="35"/>
+      <c r="U10" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V10" s="36"/>
-      <c r="W10" s="37"/>
-    </row>
-    <row r="11" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
+      <c r="W10" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
+        <v>32</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="32">
+        <v>45660</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
+      <c r="M11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="P11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R11" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>309</v>
+      </c>
       <c r="T11" s="34"/>
       <c r="U11" s="35"/>
       <c r="V11" s="36"/>
-      <c r="W11" s="37"/>
-    </row>
-    <row r="12" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
+      <c r="W11" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
+        <v>39</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="32">
+        <v>45679</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
+      <c r="M12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="P12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S12" s="34" t="s">
+        <v>145</v>
+      </c>
       <c r="T12" s="34"/>
-      <c r="U12" s="35"/>
+      <c r="U12" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V12" s="36"/>
-      <c r="W12" s="37"/>
-    </row>
-    <row r="13" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
+      <c r="W12" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
+        <v>40</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="32">
+        <v>45660</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
+      <c r="M13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R13" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>314</v>
+      </c>
       <c r="T13" s="34"/>
       <c r="U13" s="35"/>
       <c r="V13" s="36"/>
-      <c r="W13" s="37"/>
-    </row>
-    <row r="14" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
+      <c r="W13" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29">
+        <v>47</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="32">
+        <v>45621</v>
+      </c>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
+      <c r="J14" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
+      <c r="M14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="P14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>147</v>
+      </c>
       <c r="T14" s="34"/>
-      <c r="U14" s="35"/>
+      <c r="U14" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V14" s="36"/>
-      <c r="W14" s="37"/>
-    </row>
-    <row r="15" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
+      <c r="W14" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="29">
+        <v>48</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="32">
+        <v>45660</v>
+      </c>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
+      <c r="I15" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
+      <c r="M15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O15" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="P15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q15" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R15" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S15" s="34" t="s">
+        <v>316</v>
+      </c>
       <c r="T15" s="34"/>
-      <c r="U15" s="35"/>
+      <c r="U15" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V15" s="36"/>
-      <c r="W15" s="37"/>
-    </row>
-    <row r="16" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
+      <c r="W15" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="29">
+        <v>75</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
+      <c r="M16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="P16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S16" s="34" t="s">
+        <v>152</v>
+      </c>
       <c r="T16" s="34"/>
-      <c r="U16" s="35"/>
+      <c r="U16" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V16" s="36"/>
-      <c r="W16" s="37"/>
-    </row>
-    <row r="17" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
+      <c r="W16" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29">
+        <v>76</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
+      <c r="M17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O17" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="P17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q17" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R17" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S17" s="34" t="s">
+        <v>157</v>
+      </c>
       <c r="T17" s="34"/>
-      <c r="U17" s="35"/>
+      <c r="U17" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V17" s="36"/>
-      <c r="W17" s="37"/>
-    </row>
-    <row r="18" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
+      <c r="W17" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="29">
+        <v>77</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>56</v>
+      </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
       <c r="H18" s="33"/>
       <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
+      <c r="J18" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
@@ -3617,70 +4352,162 @@
       <c r="T18" s="34"/>
       <c r="U18" s="35"/>
       <c r="V18" s="36"/>
-      <c r="W18" s="37"/>
-    </row>
-    <row r="19" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34"/>
+      <c r="W18" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="29">
+        <v>78</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
+      <c r="M19" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N19" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O19" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q19" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R19" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S19" s="34" t="s">
+        <v>162</v>
+      </c>
       <c r="T19" s="34"/>
-      <c r="U19" s="35"/>
+      <c r="U19" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V19" s="36"/>
-      <c r="W19" s="37"/>
-    </row>
-    <row r="20" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
+      <c r="W19" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29">
+        <v>79</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
+      <c r="M20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="P20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R20" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S20" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="T20" s="34"/>
-      <c r="U20" s="35"/>
+      <c r="U20" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V20" s="36"/>
-      <c r="W20" s="37"/>
-    </row>
-    <row r="21" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
+      <c r="W20" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29">
+        <v>80</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
+      <c r="J21" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
@@ -3692,20 +4519,36 @@
       <c r="T21" s="34"/>
       <c r="U21" s="35"/>
       <c r="V21" s="36"/>
-      <c r="W21" s="37"/>
-    </row>
-    <row r="22" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
+      <c r="W21" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="29">
+        <v>81</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>133</v>
+      </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+      <c r="J22" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
@@ -3717,11 +4560,13 @@
       <c r="T22" s="34"/>
       <c r="U22" s="35"/>
       <c r="V22" s="36"/>
-      <c r="W22" s="37"/>
-    </row>
-    <row r="23" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W22" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>34</v>
@@ -3730,61 +4575,39 @@
         <v>38</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="32">
-        <v>45679</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="H23" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="I23" s="33" t="s">
-        <v>141</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
       <c r="J23" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L23" s="34"/>
-      <c r="M23" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N23" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O23" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="P23" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q23" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R23" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S23" s="34" t="s">
-        <v>143</v>
-      </c>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
       <c r="T23" s="34"/>
-      <c r="U23" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U23" s="35"/>
       <c r="V23" s="36"/>
       <c r="W23" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>34</v>
@@ -3793,61 +4616,39 @@
         <v>38</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="32">
-        <v>45679</v>
-      </c>
-      <c r="G24" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="H24" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>141</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
       <c r="J24" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K24" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L24" s="34"/>
-      <c r="M24" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N24" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O24" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="P24" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q24" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R24" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S24" s="34" t="s">
-        <v>145</v>
-      </c>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
       <c r="T24" s="34"/>
-      <c r="U24" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U24" s="35"/>
       <c r="V24" s="36"/>
       <c r="W24" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="29">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>34</v>
@@ -3856,55 +4657,39 @@
         <v>38</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="32">
-        <v>45621</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F25" s="32"/>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="J25" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K25" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L25" s="34"/>
-      <c r="M25" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N25" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O25" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="P25" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q25" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R25" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S25" s="34" t="s">
-        <v>147</v>
-      </c>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
       <c r="T25" s="34"/>
-      <c r="U25" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U25" s="35"/>
       <c r="V25" s="36"/>
       <c r="W25" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>34</v>
@@ -3913,22 +4698,22 @@
         <v>38</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F26" s="32">
-        <v>45621</v>
+        <v>45622</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="J26" s="34" t="s">
         <v>51</v>
@@ -3942,7 +4727,7 @@
         <v>51</v>
       </c>
       <c r="O26" s="34" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="P26" s="34" t="s">
         <v>51</v>
@@ -3954,20 +4739,18 @@
         <v>101</v>
       </c>
       <c r="S26" s="34" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="T26" s="34"/>
-      <c r="U26" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U26" s="35"/>
       <c r="V26" s="36"/>
       <c r="W26" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="29">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>34</v>
@@ -3976,37 +4759,25 @@
         <v>38</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="I27" s="33" t="s">
-        <v>155</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K27" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L27" s="34"/>
-      <c r="M27" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N27" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O27" s="34" t="s">
-        <v>156</v>
-      </c>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
       <c r="P27" s="34" t="s">
         <v>51</v>
       </c>
@@ -4017,20 +4788,18 @@
         <v>101</v>
       </c>
       <c r="S27" s="34" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="T27" s="34"/>
-      <c r="U27" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U27" s="35"/>
       <c r="V27" s="36"/>
       <c r="W27" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="29">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>34</v>
@@ -4039,10 +4808,10 @@
         <v>38</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="33"/>
@@ -4052,9 +4821,11 @@
         <v>101</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L28" s="34"/>
+        <v>112</v>
+      </c>
+      <c r="L28" s="34" t="s">
+        <v>174</v>
+      </c>
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
       <c r="O28" s="34"/>
@@ -4069,9 +4840,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="29">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>34</v>
@@ -4080,61 +4851,41 @@
         <v>38</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>160</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F29" s="32"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
       <c r="J29" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N29" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O29" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="P29" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q29" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R29" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="S29" s="34" t="s">
-        <v>162</v>
-      </c>
+      <c r="K29" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L29" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
       <c r="T29" s="34"/>
-      <c r="U29" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U29" s="35"/>
       <c r="V29" s="36"/>
       <c r="W29" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>34</v>
@@ -4143,61 +4894,41 @@
         <v>38</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G30" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="H30" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>165</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
       <c r="J30" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N30" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O30" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="P30" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q30" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R30" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="S30" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="K30" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L30" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
       <c r="T30" s="34"/>
-      <c r="U30" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U30" s="35"/>
       <c r="V30" s="36"/>
       <c r="W30" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>34</v>
@@ -4206,10 +4937,10 @@
         <v>38</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="33"/>
@@ -4219,9 +4950,11 @@
         <v>101</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L31" s="34"/>
+        <v>112</v>
+      </c>
+      <c r="L31" s="34" t="s">
+        <v>175</v>
+      </c>
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
@@ -4236,91 +4969,93 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="29">
-        <v>81</v>
-      </c>
-      <c r="B32" s="30" t="s">
+    <row r="32" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="54">
+        <v>91</v>
+      </c>
+      <c r="B32" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="34" t="s">
+      <c r="D32" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="41"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="K32" s="34" t="s">
+      <c r="K32" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="L32" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="44"/>
+      <c r="V32" s="56"/>
+      <c r="W32" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="45">
+        <v>92</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="48"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="K33" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="37" t="s">
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="50"/>
+      <c r="Q33" s="50"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="50"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="52"/>
+      <c r="W33" s="53" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="29">
-        <v>82</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K33" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="36"/>
-      <c r="W33" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="136.19999999999999" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="29">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B34" s="30" t="s">
         <v>34</v>
@@ -4329,10 +5064,10 @@
         <v>38</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="33"/>
@@ -4359,32 +5094,38 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="29">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="B35" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
+        <v>192</v>
+      </c>
+      <c r="F35" s="32">
+        <v>45690</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>195</v>
+      </c>
       <c r="J35" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K35" s="34" t="s">
-        <v>110</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K35" s="34"/>
       <c r="L35" s="34"/>
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
@@ -4397,148 +5138,136 @@
       <c r="U35" s="35"/>
       <c r="V35" s="36"/>
       <c r="W35" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="29">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="B36" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>67</v>
+        <v>196</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="F36" s="32">
-        <v>45622</v>
+        <v>45691</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="J36" s="34" t="s">
         <v>51</v>
       </c>
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
-      <c r="M36" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N36" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O36" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="P36" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q36" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R36" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S36" s="34" t="s">
-        <v>172</v>
-      </c>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="34"/>
       <c r="T36" s="34"/>
       <c r="U36" s="35"/>
       <c r="V36" s="36"/>
       <c r="W36" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="29">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="B37" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>68</v>
+        <v>201</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
+        <v>202</v>
+      </c>
+      <c r="F37" s="32">
+        <v>45691</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>205</v>
+      </c>
       <c r="J37" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K37" s="34" t="s">
-        <v>110</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K37" s="34"/>
       <c r="L37" s="34"/>
       <c r="M37" s="34"/>
       <c r="N37" s="34"/>
       <c r="O37" s="34"/>
-      <c r="P37" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q37" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R37" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S37" s="34" t="s">
-        <v>173</v>
-      </c>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="34"/>
+      <c r="R37" s="34"/>
+      <c r="S37" s="34"/>
       <c r="T37" s="34"/>
       <c r="U37" s="35"/>
       <c r="V37" s="36"/>
       <c r="W37" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="29">
-        <v>87</v>
+        <v>150</v>
       </c>
       <c r="B38" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>69</v>
+        <v>206</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
+        <v>207</v>
+      </c>
+      <c r="F38" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="H38" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>210</v>
+      </c>
       <c r="J38" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K38" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L38" s="34" t="s">
-        <v>174</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K38" s="34"/>
+      <c r="L38" s="34"/>
       <c r="M38" s="34"/>
       <c r="N38" s="34"/>
       <c r="O38" s="34"/>
@@ -4550,45 +5279,63 @@
       <c r="U38" s="35"/>
       <c r="V38" s="36"/>
       <c r="W38" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="29">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="B39" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>70</v>
+        <v>211</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
+        <v>212</v>
+      </c>
+      <c r="F39" s="32">
+        <v>45660</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>215</v>
+      </c>
       <c r="J39" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N39" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O39" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="P39" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K39" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L39" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
+      <c r="R39" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S39" s="34" t="s">
+        <v>217</v>
+      </c>
       <c r="T39" s="34"/>
       <c r="U39" s="35"/>
       <c r="V39" s="36"/>
@@ -4596,42 +5343,60 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="29">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="B40" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>71</v>
+        <v>218</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
+        <v>219</v>
+      </c>
+      <c r="F40" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="H40" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="I40" s="33" t="s">
+        <v>278</v>
+      </c>
       <c r="J40" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N40" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O40" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="P40" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K40" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L40" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
-      <c r="O40" s="34"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
-      <c r="S40" s="34"/>
+      <c r="R40" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S40" s="34" t="s">
+        <v>220</v>
+      </c>
       <c r="T40" s="34"/>
       <c r="U40" s="35"/>
       <c r="V40" s="36"/>
@@ -4639,21 +5404,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="29">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="B41" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>73</v>
+        <v>221</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="F41" s="32"/>
       <c r="G41" s="33"/>
@@ -4662,11 +5427,9 @@
       <c r="J41" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K41" s="34" t="s">
-        <v>112</v>
-      </c>
+      <c r="K41" s="34"/>
       <c r="L41" s="34" t="s">
-        <v>175</v>
+        <v>110</v>
       </c>
       <c r="M41" s="34"/>
       <c r="N41" s="34"/>
@@ -4682,42 +5445,60 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="29">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
+        <v>224</v>
+      </c>
+      <c r="F42" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="H42" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="I42" s="33" t="s">
+        <v>284</v>
+      </c>
       <c r="J42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O42" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="P42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K42" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L42" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
-      <c r="O42" s="34"/>
-      <c r="P42" s="34"/>
-      <c r="Q42" s="34"/>
-      <c r="R42" s="34"/>
-      <c r="S42" s="34"/>
+      <c r="R42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S42" s="34" t="s">
+        <v>226</v>
+      </c>
       <c r="T42" s="34"/>
       <c r="U42" s="35"/>
       <c r="V42" s="36"/>
@@ -4725,40 +5506,60 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="29">
-        <v>92</v>
+        <v>155</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>76</v>
+        <v>227</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
+        <v>228</v>
+      </c>
+      <c r="F43" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="H43" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" s="33" t="s">
+        <v>229</v>
+      </c>
       <c r="J43" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N43" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O43" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="P43" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K43" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="34"/>
-      <c r="O43" s="34"/>
-      <c r="P43" s="34"/>
-      <c r="Q43" s="34"/>
-      <c r="R43" s="34"/>
-      <c r="S43" s="34"/>
+      <c r="R43" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S43" s="34" t="s">
+        <v>226</v>
+      </c>
       <c r="T43" s="34"/>
       <c r="U43" s="35"/>
       <c r="V43" s="36"/>
@@ -4766,21 +5567,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="29">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
       <c r="F44" s="32"/>
       <c r="G44" s="33"/>
@@ -4807,391 +5608,867 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="45"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="50"/>
-      <c r="R45" s="50"/>
-      <c r="S45" s="50"/>
-      <c r="T45" s="50"/>
-      <c r="U45" s="51"/>
-      <c r="V45" s="52"/>
-      <c r="W45" s="53"/>
-    </row>
-    <row r="46" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="45"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="49"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
-      <c r="R46" s="50"/>
-      <c r="S46" s="50"/>
-      <c r="T46" s="50"/>
-      <c r="U46" s="51"/>
-      <c r="V46" s="52"/>
-      <c r="W46" s="53"/>
-    </row>
-    <row r="47" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="54">
+    <row r="45" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="29">
+        <v>157</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" s="32"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K45" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L45" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="34"/>
+      <c r="P45" s="34"/>
+      <c r="Q45" s="34"/>
+      <c r="R45" s="34"/>
+      <c r="S45" s="34"/>
+      <c r="T45" s="34"/>
+      <c r="U45" s="35"/>
+      <c r="V45" s="36"/>
+      <c r="W45" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="29">
+        <v>158</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="F46" s="32"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K46" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
+      <c r="P46" s="34"/>
+      <c r="Q46" s="34"/>
+      <c r="R46" s="34"/>
+      <c r="S46" s="34"/>
+      <c r="T46" s="34"/>
+      <c r="U46" s="35"/>
+      <c r="V46" s="36"/>
+      <c r="W46" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="29">
+        <v>159</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F47" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="H47" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="I47" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O47" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="P47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q47" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S47" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="T47" s="34"/>
+      <c r="U47" s="35"/>
+      <c r="V47" s="36"/>
+      <c r="W47" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="29">
+        <v>160</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="F48" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="H48" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="I48" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="J48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O48" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="P48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S48" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="T48" s="34"/>
+      <c r="U48" s="35"/>
+      <c r="V48" s="36"/>
+      <c r="W48" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="29">
+        <v>161</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="F49" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="H49" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="I49" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="J49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O49" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="P49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S49" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="T49" s="34"/>
+      <c r="U49" s="35"/>
+      <c r="V49" s="36"/>
+      <c r="W49" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="29">
+        <v>162</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="F50" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="H50" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="I50" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="J50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O50" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="P50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S50" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="T50" s="34"/>
+      <c r="U50" s="35"/>
+      <c r="V50" s="36"/>
+      <c r="W50" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="29">
+        <v>163</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="F51" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G51" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="H51" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="I51" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="J51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O51" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="P51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S51" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="T51" s="34"/>
+      <c r="U51" s="35"/>
+      <c r="V51" s="36"/>
+      <c r="W51" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="29">
+        <v>164</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K52" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L52" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="M52" s="34"/>
+      <c r="N52" s="34"/>
+      <c r="O52" s="34"/>
+      <c r="P52" s="34"/>
+      <c r="Q52" s="34"/>
+      <c r="R52" s="34"/>
+      <c r="S52" s="34"/>
+      <c r="T52" s="34"/>
+      <c r="U52" s="35"/>
+      <c r="V52" s="36"/>
+      <c r="W52" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="29">
+        <v>165</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="F53" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="H53" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="I53" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="J53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O53" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="P53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S53" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="T53" s="34"/>
+      <c r="U53" s="35"/>
+      <c r="V53" s="36"/>
+      <c r="W53" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="29">
+        <v>166</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K54" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L54" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M54" s="34"/>
+      <c r="N54" s="34"/>
+      <c r="O54" s="34"/>
+      <c r="P54" s="34"/>
+      <c r="Q54" s="34"/>
+      <c r="R54" s="34"/>
+      <c r="S54" s="34"/>
+      <c r="T54" s="34"/>
+      <c r="U54" s="35"/>
+      <c r="V54" s="36"/>
+      <c r="W54" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="29">
+        <v>167</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="F55" s="32">
+        <v>45692</v>
+      </c>
+      <c r="G55" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="H55" s="33" t="s">
+        <v>304</v>
+      </c>
+      <c r="I55" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="J55" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="34"/>
+      <c r="N55" s="34"/>
+      <c r="O55" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="P55" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q55" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R55" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S55" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="T55" s="34"/>
+      <c r="U55" s="35"/>
+      <c r="V55" s="36"/>
+      <c r="W55" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="29">
+        <v>168</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F56" s="32">
+        <v>45700</v>
+      </c>
+      <c r="G56" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="H56" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="I56" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="J56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K56" s="34"/>
+      <c r="L56" s="34"/>
+      <c r="M56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O56" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="P56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S56" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="T56" s="34"/>
+      <c r="U56" s="35"/>
+      <c r="V56" s="36"/>
+      <c r="W56" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="29">
+        <v>169</v>
+      </c>
+      <c r="B57" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="F57" s="32">
+        <v>45700</v>
+      </c>
+      <c r="G57" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="H57" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="I57" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="J57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O57" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="P57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S57" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="T57" s="34"/>
+      <c r="U57" s="35"/>
+      <c r="V57" s="36"/>
+      <c r="W57" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="29">
+        <v>374</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="F58" s="32">
+        <v>45700</v>
+      </c>
+      <c r="G58" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="H58" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="I58" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="J58" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K58" s="34"/>
+      <c r="L58" s="34"/>
+      <c r="M58" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="N58" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="O58" s="34"/>
+      <c r="P58" s="34"/>
+      <c r="Q58" s="34"/>
+      <c r="R58" s="34"/>
+      <c r="S58" s="34"/>
+      <c r="T58" s="34"/>
+      <c r="U58" s="35"/>
+      <c r="V58" s="36"/>
+      <c r="W58" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="136.19999999999999" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="29">
         <v>446</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B59" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="55" t="s">
+      <c r="C59" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D59" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E59" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="F47" s="41">
+      <c r="F59" s="32">
         <v>45685</v>
       </c>
-      <c r="G47" s="42" t="s">
+      <c r="G59" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H47" s="42" t="s">
+      <c r="H59" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="I47" s="42" t="s">
+      <c r="I59" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="J47" s="43" t="s">
+      <c r="J59" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="43"/>
-      <c r="S47" s="43"/>
-      <c r="T47" s="43"/>
-      <c r="U47" s="44"/>
-      <c r="V47" s="56"/>
-      <c r="W47" s="38" t="s">
+      <c r="K59" s="34"/>
+      <c r="L59" s="34"/>
+      <c r="M59" s="34"/>
+      <c r="N59" s="34"/>
+      <c r="O59" s="34"/>
+      <c r="P59" s="34"/>
+      <c r="Q59" s="34"/>
+      <c r="R59" s="34"/>
+      <c r="S59" s="34"/>
+      <c r="T59" s="34"/>
+      <c r="U59" s="35"/>
+      <c r="V59" s="36"/>
+      <c r="W59" s="37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="45">
+    <row r="60" spans="1:23" ht="136.19999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="29">
         <v>447</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B60" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C60" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="46" t="s">
+      <c r="D60" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="47" t="s">
+      <c r="E60" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="48">
+      <c r="F60" s="32">
         <v>45685</v>
       </c>
-      <c r="G48" s="49" t="s">
+      <c r="G60" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="H48" s="49" t="s">
+      <c r="H60" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="I48" s="49" t="s">
+      <c r="I60" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="J48" s="50" t="s">
+      <c r="J60" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
-      <c r="M48" s="50"/>
-      <c r="N48" s="50"/>
-      <c r="O48" s="50"/>
-      <c r="P48" s="50"/>
-      <c r="Q48" s="50"/>
-      <c r="R48" s="50"/>
-      <c r="S48" s="50"/>
-      <c r="T48" s="50"/>
-      <c r="U48" s="51"/>
-      <c r="V48" s="52"/>
-      <c r="W48" s="53" t="s">
+      <c r="K60" s="34"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="34"/>
+      <c r="N60" s="34"/>
+      <c r="O60" s="34"/>
+      <c r="P60" s="34"/>
+      <c r="Q60" s="34"/>
+      <c r="R60" s="34"/>
+      <c r="S60" s="34"/>
+      <c r="T60" s="34"/>
+      <c r="U60" s="35"/>
+      <c r="V60" s="36"/>
+      <c r="W60" s="37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="7"/>
-      <c r="T49" s="7"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="9"/>
-    </row>
-    <row r="50" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="7"/>
-      <c r="S50" s="7"/>
-      <c r="T50" s="7"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="9"/>
-    </row>
-    <row r="51" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
-      <c r="S51" s="7"/>
-      <c r="T51" s="7"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="9"/>
-    </row>
-    <row r="52" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="2"/>
-      <c r="W52" s="9"/>
-    </row>
-    <row r="53" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
-      <c r="U53" s="8"/>
-      <c r="V53" s="2"/>
-      <c r="W53" s="9"/>
-    </row>
-    <row r="54" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="7"/>
-      <c r="T54" s="7"/>
-      <c r="U54" s="8"/>
-      <c r="V54" s="2"/>
-      <c r="W54" s="9"/>
-    </row>
-    <row r="55" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-      <c r="U55" s="8"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="9"/>
-    </row>
-    <row r="56" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
-      <c r="U56" s="8"/>
-      <c r="V56" s="2"/>
-      <c r="W56" s="9"/>
-    </row>
-    <row r="57" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-      <c r="U57" s="8"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="9"/>
-    </row>
-    <row r="58" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="7"/>
-      <c r="T58" s="7"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="2"/>
-      <c r="W58" s="9"/>
-    </row>
-    <row r="59" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="7"/>
-      <c r="T59" s="7"/>
-      <c r="U59" s="8"/>
-      <c r="V59" s="2"/>
-      <c r="W59" s="9"/>
-    </row>
-    <row r="60" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="7"/>
-      <c r="S60" s="7"/>
-      <c r="T60" s="7"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="2"/>
-      <c r="W60" s="9"/>
-    </row>
-    <row r="61" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
@@ -5211,7 +6488,7 @@
       <c r="V61" s="2"/>
       <c r="W61" s="9"/>
     </row>
-    <row r="62" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
@@ -5231,7 +6508,7 @@
       <c r="V62" s="2"/>
       <c r="W62" s="9"/>
     </row>
-    <row r="63" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
@@ -5251,7 +6528,7 @@
       <c r="V63" s="2"/>
       <c r="W63" s="9"/>
     </row>
-    <row r="64" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
@@ -8052,270 +9329,66 @@
       <c r="W203" s="9"/>
     </row>
     <row r="204" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F204" s="6"/>
-      <c r="G204" s="6"/>
-      <c r="H204" s="6"/>
-      <c r="I204" s="6"/>
-      <c r="J204" s="7"/>
-      <c r="K204" s="7"/>
-      <c r="L204" s="7"/>
-      <c r="M204" s="7"/>
-      <c r="N204" s="7"/>
-      <c r="O204" s="7"/>
-      <c r="P204" s="7"/>
-      <c r="Q204" s="7"/>
-      <c r="R204" s="7"/>
-      <c r="S204" s="7"/>
-      <c r="T204" s="7"/>
-      <c r="U204" s="8"/>
-      <c r="V204" s="2"/>
-      <c r="W204" s="9"/>
+      <c r="W204" s="7"/>
     </row>
     <row r="205" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F205" s="6"/>
-      <c r="G205" s="6"/>
-      <c r="H205" s="6"/>
-      <c r="I205" s="6"/>
-      <c r="J205" s="7"/>
-      <c r="K205" s="7"/>
-      <c r="L205" s="7"/>
-      <c r="M205" s="7"/>
-      <c r="N205" s="7"/>
-      <c r="O205" s="7"/>
-      <c r="P205" s="7"/>
-      <c r="Q205" s="7"/>
-      <c r="R205" s="7"/>
-      <c r="S205" s="7"/>
-      <c r="T205" s="7"/>
-      <c r="U205" s="8"/>
-      <c r="V205" s="2"/>
-      <c r="W205" s="9"/>
+      <c r="W205" s="7"/>
     </row>
     <row r="206" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F206" s="6"/>
-      <c r="G206" s="6"/>
-      <c r="H206" s="6"/>
-      <c r="I206" s="6"/>
-      <c r="J206" s="7"/>
-      <c r="K206" s="7"/>
-      <c r="L206" s="7"/>
-      <c r="M206" s="7"/>
-      <c r="N206" s="7"/>
-      <c r="O206" s="7"/>
-      <c r="P206" s="7"/>
-      <c r="Q206" s="7"/>
-      <c r="R206" s="7"/>
-      <c r="S206" s="7"/>
-      <c r="T206" s="7"/>
-      <c r="U206" s="8"/>
-      <c r="V206" s="2"/>
-      <c r="W206" s="9"/>
+      <c r="W206" s="7"/>
     </row>
     <row r="207" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F207" s="6"/>
-      <c r="G207" s="6"/>
-      <c r="H207" s="6"/>
-      <c r="I207" s="6"/>
-      <c r="J207" s="7"/>
-      <c r="K207" s="7"/>
-      <c r="L207" s="7"/>
-      <c r="M207" s="7"/>
-      <c r="N207" s="7"/>
-      <c r="O207" s="7"/>
-      <c r="P207" s="7"/>
-      <c r="Q207" s="7"/>
-      <c r="R207" s="7"/>
-      <c r="S207" s="7"/>
-      <c r="T207" s="7"/>
-      <c r="U207" s="8"/>
-      <c r="V207" s="2"/>
-      <c r="W207" s="9"/>
+      <c r="W207" s="7"/>
     </row>
     <row r="208" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F208" s="6"/>
-      <c r="G208" s="6"/>
-      <c r="H208" s="6"/>
-      <c r="I208" s="6"/>
-      <c r="J208" s="7"/>
-      <c r="K208" s="7"/>
-      <c r="L208" s="7"/>
-      <c r="M208" s="7"/>
-      <c r="N208" s="7"/>
-      <c r="O208" s="7"/>
-      <c r="P208" s="7"/>
-      <c r="Q208" s="7"/>
-      <c r="R208" s="7"/>
-      <c r="S208" s="7"/>
-      <c r="T208" s="7"/>
-      <c r="U208" s="8"/>
-      <c r="V208" s="2"/>
-      <c r="W208" s="9"/>
-    </row>
-    <row r="209" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F209" s="6"/>
-      <c r="G209" s="6"/>
-      <c r="H209" s="6"/>
-      <c r="I209" s="6"/>
-      <c r="J209" s="7"/>
-      <c r="K209" s="7"/>
-      <c r="L209" s="7"/>
-      <c r="M209" s="7"/>
-      <c r="N209" s="7"/>
-      <c r="O209" s="7"/>
-      <c r="P209" s="7"/>
-      <c r="Q209" s="7"/>
-      <c r="R209" s="7"/>
-      <c r="S209" s="7"/>
-      <c r="T209" s="7"/>
-      <c r="U209" s="8"/>
-      <c r="V209" s="2"/>
-      <c r="W209" s="9"/>
-    </row>
-    <row r="210" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F210" s="6"/>
-      <c r="G210" s="6"/>
-      <c r="H210" s="6"/>
-      <c r="I210" s="6"/>
-      <c r="J210" s="7"/>
-      <c r="K210" s="7"/>
-      <c r="L210" s="7"/>
-      <c r="M210" s="7"/>
-      <c r="N210" s="7"/>
-      <c r="O210" s="7"/>
-      <c r="P210" s="7"/>
-      <c r="Q210" s="7"/>
-      <c r="R210" s="7"/>
-      <c r="S210" s="7"/>
-      <c r="T210" s="7"/>
-      <c r="U210" s="8"/>
-      <c r="V210" s="2"/>
-      <c r="W210" s="9"/>
-    </row>
-    <row r="211" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F211" s="6"/>
-      <c r="G211" s="6"/>
-      <c r="H211" s="6"/>
-      <c r="I211" s="6"/>
-      <c r="J211" s="7"/>
-      <c r="K211" s="7"/>
-      <c r="L211" s="7"/>
-      <c r="M211" s="7"/>
-      <c r="N211" s="7"/>
-      <c r="O211" s="7"/>
-      <c r="P211" s="7"/>
-      <c r="Q211" s="7"/>
-      <c r="R211" s="7"/>
-      <c r="S211" s="7"/>
-      <c r="T211" s="7"/>
-      <c r="U211" s="8"/>
-      <c r="V211" s="2"/>
-      <c r="W211" s="9"/>
-    </row>
-    <row r="212" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F212" s="6"/>
-      <c r="G212" s="6"/>
-      <c r="H212" s="6"/>
-      <c r="I212" s="6"/>
-      <c r="J212" s="7"/>
-      <c r="K212" s="7"/>
-      <c r="L212" s="7"/>
-      <c r="M212" s="7"/>
-      <c r="N212" s="7"/>
-      <c r="O212" s="7"/>
-      <c r="P212" s="7"/>
-      <c r="Q212" s="7"/>
-      <c r="R212" s="7"/>
-      <c r="S212" s="7"/>
-      <c r="T212" s="7"/>
-      <c r="U212" s="8"/>
-      <c r="V212" s="2"/>
-      <c r="W212" s="9"/>
-    </row>
-    <row r="213" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F213" s="6"/>
-      <c r="G213" s="6"/>
-      <c r="H213" s="6"/>
-      <c r="I213" s="6"/>
-      <c r="J213" s="7"/>
-      <c r="K213" s="7"/>
-      <c r="L213" s="7"/>
-      <c r="M213" s="7"/>
-      <c r="N213" s="7"/>
-      <c r="O213" s="7"/>
-      <c r="P213" s="7"/>
-      <c r="Q213" s="7"/>
-      <c r="R213" s="7"/>
-      <c r="S213" s="7"/>
-      <c r="T213" s="7"/>
-      <c r="U213" s="8"/>
-      <c r="V213" s="2"/>
-      <c r="W213" s="9"/>
-    </row>
-    <row r="214" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F214" s="6"/>
-      <c r="G214" s="6"/>
-      <c r="H214" s="6"/>
-      <c r="I214" s="6"/>
-      <c r="J214" s="7"/>
-      <c r="K214" s="7"/>
-      <c r="L214" s="7"/>
-      <c r="M214" s="7"/>
-      <c r="N214" s="7"/>
-      <c r="O214" s="7"/>
-      <c r="P214" s="7"/>
-      <c r="Q214" s="7"/>
-      <c r="R214" s="7"/>
-      <c r="S214" s="7"/>
-      <c r="T214" s="7"/>
-      <c r="U214" s="8"/>
-      <c r="V214" s="2"/>
-      <c r="W214" s="9"/>
-    </row>
-    <row r="215" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F215" s="6"/>
-      <c r="G215" s="6"/>
-      <c r="H215" s="6"/>
-      <c r="I215" s="6"/>
-      <c r="J215" s="7"/>
-      <c r="K215" s="7"/>
-      <c r="L215" s="7"/>
-      <c r="M215" s="7"/>
-      <c r="N215" s="7"/>
-      <c r="O215" s="7"/>
-      <c r="P215" s="7"/>
-      <c r="Q215" s="7"/>
-      <c r="R215" s="7"/>
-      <c r="S215" s="7"/>
-      <c r="T215" s="7"/>
-      <c r="U215" s="8"/>
-      <c r="V215" s="2"/>
-      <c r="W215" s="9"/>
-    </row>
-    <row r="216" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W208" s="7"/>
+    </row>
+    <row r="209" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W209" s="7"/>
+    </row>
+    <row r="210" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W210" s="7"/>
+    </row>
+    <row r="211" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W211" s="7"/>
+    </row>
+    <row r="212" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W212" s="7"/>
+    </row>
+    <row r="213" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W213" s="7"/>
+    </row>
+    <row r="214" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W214" s="7"/>
+    </row>
+    <row r="215" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W215" s="7"/>
+    </row>
+    <row r="216" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W216" s="7"/>
     </row>
-    <row r="217" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W217" s="7"/>
     </row>
-    <row r="218" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W218" s="7"/>
     </row>
-    <row r="219" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W219" s="7"/>
     </row>
-    <row r="220" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W220" s="7"/>
     </row>
-    <row r="221" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W221" s="7"/>
     </row>
-    <row r="222" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W222" s="7"/>
     </row>
-    <row r="223" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W223" s="7"/>
     </row>
-    <row r="224" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W224" s="7"/>
     </row>
     <row r="225" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -9506,49 +10579,16 @@
     <row r="620" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W620" s="7"/>
     </row>
-    <row r="621" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W621" s="7"/>
-    </row>
-    <row r="622" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W622" s="7"/>
-    </row>
-    <row r="623" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W623" s="7"/>
-    </row>
-    <row r="624" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W624" s="7"/>
-    </row>
-    <row r="625" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W625" s="7"/>
-    </row>
-    <row r="626" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W626" s="7"/>
-    </row>
-    <row r="627" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W627" s="7"/>
-    </row>
-    <row r="628" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W628" s="7"/>
-    </row>
-    <row r="629" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W629" s="7"/>
-    </row>
-    <row r="630" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W630" s="7"/>
-    </row>
-    <row r="631" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W631" s="7"/>
-    </row>
-    <row r="632" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W632" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A9:W48" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <autoFilter ref="A9:W60" xr:uid="{00000000-0001-0000-0200-000000000000}">
     <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters>
+        <filter val="RSA"/>
+      </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:W60">
+      <sortCondition ref="A9:A60"/>
+    </sortState>
   </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
@@ -9561,8 +10601,8 @@
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -9570,19 +10610,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P10:R48 J10:J48 M10:N48</xm:sqref>
+          <xm:sqref>M10:N33 P10:R33 J10:J33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T10:T48</xm:sqref>
+          <xm:sqref>T10:T33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K48</xm:sqref>
+          <xm:sqref>K10:K33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9651,7 +10691,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9685,7 +10725,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -9699,7 +10739,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>37</v>
       </c>
@@ -9713,7 +10753,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
@@ -9727,7 +10767,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
@@ -9741,7 +10781,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -9755,7 +10795,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -9769,7 +10809,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -9783,7 +10823,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -9797,7 +10837,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>96</v>
       </c>
@@ -9811,7 +10851,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'upstream/main'"
This reverts commit 10154d2b0e1a98dd5f758dec3a348900274d0e39, reversing
changes made to dee19b411b58b503f54953dba336d34136844332.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\GENIUSRL\POCR\1.0.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666B7BF1-F8A2-49BB-9E75-D9EA26702EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76930517-3941-41AA-BC81-025ADBF1F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$48</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="191">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -828,437 +828,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.d63c6b2c88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
-  </si>
-  <si>
-    <t>2025-02-02T18:45:59Z</t>
-  </si>
-  <si>
-    <t>4e7664ac1c33c161</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.cb0f4e1eb9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
-  </si>
-  <si>
-    <t>2025-02-03T16:58:24Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.6c550f02e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8555dbcac8c5751b</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
-  </si>
-  <si>
-    <t>2025-02-03T17:35:26Z</t>
-  </si>
-  <si>
-    <t>4adf0eb3a689a290</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.562d3ce0fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
-  </si>
-  <si>
-    <t>2025-02-04T12:41:28Z</t>
-  </si>
-  <si>
-    <t>2f6f11739b90d6e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.60ce93b68e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2025-01-03T14:28:58Z</t>
-  </si>
-  <si>
-    <t>f0abc2dec788a4c3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.e18d2ba9e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Errore di sintassi: ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
-  </si>
-  <si>
-    <t>L'errore viene gestito a livello di applicazione alla produzione del referto</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>L'errore viene gestito dall'applicaizone con il controllo del codice fiscale</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT7_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>Prima di effettuare l'invio viene validato il file e controllato</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.23195b441f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.cc9a571001^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Il controllo del file xml viene eseguito prima dell'invio</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>c4adc4670c76ce65</t>
-  </si>
-  <si>
-    <t>Errore gestito dallìapplicaizone, controllando prima la valiazione</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>[ERRORE-b4| Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento 'text'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>Non è possibile inviare se la sezione è vuota, controllo dell'applicazione</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>Controllo dei campi obbligaotri e verifica prima dell'invio</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene gestito l'obbligatorietà dei valori</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>l campo effectivetime/low ha sempre un valore di default, se non è presente la data perché non è disponbile (es. il paziente non ricorda) allora è presente il valore @nullFlavor = “UNK”.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>62d028544054dd72</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.9d48385b32476688046faa7dd456a15a3e45daecc0a272d177dc29b38d348637.a2aef11856^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[ERRORE-b36| Sezione Storia Clinica: l'elemento entry/organizer/subject/relatedSubject deve avere l'attributo @classCode='PRS' e deve contenere l'elemento 'code'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>Gestito dall'aplicaizone</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Gestito dall'applicazione campo obbligatorio</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
-  </si>
-  <si>
-    <t>"Errore semantico. [ERRORE-44| Il codice fiscale '0012132145' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]"</t>
-  </si>
-  <si>
-    <t>a83bd16efcf9de0d</t>
-  </si>
-  <si>
-    <t>workflowInstanceId":"2.16.840.1.113883.2.9.2.120.4.4.758ddd9e38865de2ce747bb084caaf34b3f04d250edf0f79b491b5322fe0862f.930b68af3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T15:30:08Z</t>
-  </si>
-  <si>
-    <t>b2346e487feac030</t>
-  </si>
-  <si>
-    <t>2025-02-04T15:36:52Z</t>
-  </si>
-  <si>
-    <t>da883b8cd9c0542e</t>
-  </si>
-  <si>
-    <t>2025-02-04T16:33:05Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.c04afd54de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Errore di sintassi. ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'priorityCode'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected</t>
-  </si>
-  <si>
-    <t>2025-02-04T16:58:36Z</t>
-  </si>
-  <si>
-    <t>860af4e087971bb6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.6b9df4a85d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.,ERROR: -1,-1 cvc-datatype-valid.1.2.3: '' is not a valid value of union type 'uid'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'codeSystem' on element 'code' is not valid with respect to its type, 'uid'."</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:09:57Z</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:15:09Z</t>
-  </si>
-  <si>
-    <t>e34b8cb72eda5b7d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ccc318dc89^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:21:17Z</t>
-  </si>
-  <si>
-    <t>6cb600782a006772</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.59c944599d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:36:02Z</t>
-  </si>
-  <si>
-    <t>8e55629de097fdb4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.4a9ca2fe7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:51:45Z</t>
-  </si>
-  <si>
-    <t>"[ERRORE-b53| Sotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]"</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:55:47Z</t>
-  </si>
-  <si>
-    <t>b159f3ef01bdef63</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.0a2f34d7b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
-  </si>
-  <si>
-    <t>2025-01-03T12:48:01Z</t>
-  </si>
-  <si>
-    <t>8c22d910bd845ebc</t>
-  </si>
-  <si>
-    <t>Viene segnalato un errore di token non valido all'utente</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
-  </si>
-  <si>
-    <t>2025-01-03T13:07:58Z</t>
-  </si>
-  <si>
-    <t>5461d8a35b4a54f7</t>
-  </si>
-  <si>
-    <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
-  </si>
-  <si>
-    <t>Viene fornito un messaggio di errore all'utente, campi token non validi</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_RSA_TIMEOUT</t>
-  </si>
-  <si>
-    <t>timeout servizio FSE</t>
-  </si>
-  <si>
-    <t>2025-02-12T13:44:10Z</t>
-  </si>
-  <si>
-    <t>667b3f100bd7d00b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ca19dd635e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[ERRORE-b21| Sezione Quesito Diagnostico: l'elemento entry/observation/code deve avere l'attributo @code='29298-7' e l'attributo @codeSystem='2.16.840.1.113883.6.1'],[ERRORE-b53| Sotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
-  </si>
-  <si>
-    <t>2025-02-12T13:49:51Z</t>
-  </si>
-  <si>
-    <t>2025-02-12T14:28:16Z</t>
-  </si>
-  <si>
-    <t>e9124089694e6dcb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0ff4781c1f9e6a8fb839e1fec3454cd93f14291baec87f8c5b1351f304ad89fb.ffcc1560c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +1957,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3534,13 +3103,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:W620"/>
+  <dimension ref="A1:W632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3825,522 +3394,218 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
-        <v>31</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="32">
-        <v>45679</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="J10" s="34" t="s">
-        <v>51</v>
-      </c>
+    <row r="10" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="P10" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R10" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S10" s="34" t="s">
-        <v>143</v>
-      </c>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
       <c r="T10" s="34"/>
-      <c r="U10" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U10" s="35"/>
       <c r="V10" s="36"/>
-      <c r="W10" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="29">
-        <v>32</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>306</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="32">
-        <v>45660</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>307</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>308</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="J11" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W10" s="37"/>
+    </row>
+    <row r="11" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="P11" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R11" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S11" s="34" t="s">
-        <v>309</v>
-      </c>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
       <c r="T11" s="34"/>
       <c r="U11" s="35"/>
       <c r="V11" s="36"/>
-      <c r="W11" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
-        <v>39</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="32">
-        <v>45679</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="I12" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="J12" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W11" s="37"/>
+    </row>
+    <row r="12" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O12" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="P12" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q12" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R12" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S12" s="34" t="s">
-        <v>145</v>
-      </c>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
       <c r="T12" s="34"/>
-      <c r="U12" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U12" s="35"/>
       <c r="V12" s="36"/>
-      <c r="W12" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29">
-        <v>40</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>310</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="32">
-        <v>45660</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W12" s="37"/>
+    </row>
+    <row r="13" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
-      <c r="M13" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N13" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="34" t="s">
-        <v>313</v>
-      </c>
-      <c r="P13" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q13" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R13" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S13" s="34" t="s">
-        <v>314</v>
-      </c>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
       <c r="T13" s="34"/>
       <c r="U13" s="35"/>
       <c r="V13" s="36"/>
-      <c r="W13" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29">
-        <v>47</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="32">
-        <v>45621</v>
-      </c>
+      <c r="W13" s="37"/>
+    </row>
+    <row r="14" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
-      <c r="J14" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
-      <c r="M14" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O14" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="P14" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R14" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S14" s="34" t="s">
-        <v>147</v>
-      </c>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
       <c r="T14" s="34"/>
-      <c r="U14" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U14" s="35"/>
       <c r="V14" s="36"/>
-      <c r="W14" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="29">
-        <v>48</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="32">
-        <v>45660</v>
-      </c>
+      <c r="W14" s="37"/>
+    </row>
+    <row r="15" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
-      <c r="I15" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="J15" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="M15" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N15" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O15" s="34" t="s">
-        <v>316</v>
-      </c>
-      <c r="P15" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q15" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R15" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S15" s="34" t="s">
-        <v>316</v>
-      </c>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
       <c r="T15" s="34"/>
-      <c r="U15" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U15" s="35"/>
       <c r="V15" s="36"/>
-      <c r="W15" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29">
-        <v>75</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="J16" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W15" s="37"/>
+    </row>
+    <row r="16" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
-      <c r="M16" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O16" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="P16" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q16" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R16" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S16" s="34" t="s">
-        <v>152</v>
-      </c>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
       <c r="T16" s="34"/>
-      <c r="U16" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U16" s="35"/>
       <c r="V16" s="36"/>
-      <c r="W16" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29">
-        <v>76</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="J17" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W16" s="37"/>
+    </row>
+    <row r="17" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-      <c r="M17" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O17" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="P17" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q17" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R17" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S17" s="34" t="s">
-        <v>157</v>
-      </c>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
       <c r="T17" s="34"/>
-      <c r="U17" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U17" s="35"/>
       <c r="V17" s="36"/>
-      <c r="W17" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="29">
-        <v>77</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="W17" s="37"/>
+    </row>
+    <row r="18" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
       <c r="H18" s="33"/>
       <c r="I18" s="33"/>
-      <c r="J18" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" s="34" t="s">
-        <v>110</v>
-      </c>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
@@ -4352,162 +3617,70 @@
       <c r="T18" s="34"/>
       <c r="U18" s="35"/>
       <c r="V18" s="36"/>
-      <c r="W18" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="29">
-        <v>78</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W18" s="37"/>
+    </row>
+    <row r="19" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N19" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O19" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="P19" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q19" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R19" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S19" s="34" t="s">
-        <v>162</v>
-      </c>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
       <c r="T19" s="34"/>
-      <c r="U19" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U19" s="35"/>
       <c r="V19" s="36"/>
-      <c r="W19" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29">
-        <v>79</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="32">
-        <v>45621</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>51</v>
-      </c>
+      <c r="W19" s="37"/>
+    </row>
+    <row r="20" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="34"/>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
-      <c r="M20" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N20" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O20" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="P20" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q20" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R20" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S20" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
       <c r="T20" s="34"/>
-      <c r="U20" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="U20" s="35"/>
       <c r="V20" s="36"/>
-      <c r="W20" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="29">
-        <v>80</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>132</v>
-      </c>
+      <c r="W20" s="37"/>
+    </row>
+    <row r="21" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
-      <c r="J21" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K21" s="34" t="s">
-        <v>110</v>
-      </c>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
@@ -4519,36 +3692,20 @@
       <c r="T21" s="34"/>
       <c r="U21" s="35"/>
       <c r="V21" s="36"/>
-      <c r="W21" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="29">
-        <v>81</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>133</v>
-      </c>
+      <c r="W21" s="37"/>
+    </row>
+    <row r="22" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="29"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
-      <c r="J22" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K22" s="34" t="s">
-        <v>110</v>
-      </c>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
@@ -4560,13 +3717,11 @@
       <c r="T22" s="34"/>
       <c r="U22" s="35"/>
       <c r="V22" s="36"/>
-      <c r="W22" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W22" s="37"/>
+    </row>
+    <row r="23" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>34</v>
@@ -4575,39 +3730,61 @@
         <v>38</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
+        <v>44</v>
+      </c>
+      <c r="F23" s="32">
+        <v>45679</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>141</v>
+      </c>
       <c r="J23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O23" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="P23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q23" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K23" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
+      <c r="R23" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S23" s="34" t="s">
+        <v>143</v>
+      </c>
       <c r="T23" s="34"/>
-      <c r="U23" s="35"/>
+      <c r="U23" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V23" s="36"/>
       <c r="W23" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>34</v>
@@ -4616,39 +3793,61 @@
         <v>38</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
+        <v>49</v>
+      </c>
+      <c r="F24" s="32">
+        <v>45679</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>141</v>
+      </c>
       <c r="J24" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="P24" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q24" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K24" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
+      <c r="R24" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S24" s="34" t="s">
+        <v>145</v>
+      </c>
       <c r="T24" s="34"/>
-      <c r="U24" s="35"/>
+      <c r="U24" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V24" s="36"/>
       <c r="W24" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="29">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>34</v>
@@ -4657,39 +3856,55 @@
         <v>38</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="32"/>
+        <v>113</v>
+      </c>
+      <c r="F25" s="32">
+        <v>45621</v>
+      </c>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="J25" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O25" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="P25" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q25" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K25" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
+      <c r="R25" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S25" s="34" t="s">
+        <v>147</v>
+      </c>
       <c r="T25" s="34"/>
-      <c r="U25" s="35"/>
+      <c r="U25" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V25" s="36"/>
       <c r="W25" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>34</v>
@@ -4698,22 +3913,22 @@
         <v>38</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F26" s="32">
-        <v>45622</v>
+        <v>45621</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="J26" s="34" t="s">
         <v>51</v>
@@ -4727,7 +3942,7 @@
         <v>51</v>
       </c>
       <c r="O26" s="34" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="P26" s="34" t="s">
         <v>51</v>
@@ -4739,18 +3954,20 @@
         <v>101</v>
       </c>
       <c r="S26" s="34" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="T26" s="34"/>
-      <c r="U26" s="35"/>
+      <c r="U26" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V26" s="36"/>
       <c r="W26" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="29">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>34</v>
@@ -4759,25 +3976,37 @@
         <v>38</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
+        <v>130</v>
+      </c>
+      <c r="F27" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>155</v>
+      </c>
       <c r="J27" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K27" s="34" t="s">
-        <v>110</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K27" s="34"/>
       <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
+      <c r="M27" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O27" s="34" t="s">
+        <v>156</v>
+      </c>
       <c r="P27" s="34" t="s">
         <v>51</v>
       </c>
@@ -4788,18 +4017,20 @@
         <v>101</v>
       </c>
       <c r="S27" s="34" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="T27" s="34"/>
-      <c r="U27" s="35"/>
+      <c r="U27" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V27" s="36"/>
       <c r="W27" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="29">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>34</v>
@@ -4808,10 +4039,10 @@
         <v>38</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="33"/>
@@ -4821,11 +4052,9 @@
         <v>101</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L28" s="34" t="s">
-        <v>174</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="L28" s="34"/>
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
       <c r="O28" s="34"/>
@@ -4840,9 +4069,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="29">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>34</v>
@@ -4851,41 +4080,61 @@
         <v>38</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
+        <v>58</v>
+      </c>
+      <c r="F29" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>160</v>
+      </c>
       <c r="J29" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N29" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O29" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="P29" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q29" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R29" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K29" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L29" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34"/>
+      <c r="S29" s="34" t="s">
+        <v>162</v>
+      </c>
       <c r="T29" s="34"/>
-      <c r="U29" s="35"/>
+      <c r="U29" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V29" s="36"/>
       <c r="W29" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>34</v>
@@ -4894,41 +4143,61 @@
         <v>38</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
+        <v>131</v>
+      </c>
+      <c r="F30" s="32">
+        <v>45621</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>165</v>
+      </c>
       <c r="J30" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N30" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O30" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="P30" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q30" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R30" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K30" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L30" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34"/>
+      <c r="S30" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="T30" s="34"/>
-      <c r="U30" s="35"/>
+      <c r="U30" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="V30" s="36"/>
       <c r="W30" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>34</v>
@@ -4937,10 +4206,10 @@
         <v>38</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="33"/>
@@ -4950,11 +4219,9 @@
         <v>101</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L31" s="34" t="s">
-        <v>175</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="L31" s="34"/>
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
@@ -4969,93 +4236,91 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="54">
-        <v>91</v>
-      </c>
-      <c r="B32" s="55" t="s">
+    <row r="32" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="29">
+        <v>81</v>
+      </c>
+      <c r="B32" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="43" t="s">
+      <c r="D32" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K32" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="L32" s="43" t="s">
-        <v>177</v>
-      </c>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="43"/>
-      <c r="U32" s="44"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="38" t="s">
+      <c r="K32" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="35"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="162.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="45">
-        <v>92</v>
-      </c>
-      <c r="B33" s="46" t="s">
+    <row r="33" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="29">
+        <v>82</v>
+      </c>
+      <c r="B33" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="48"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="50" t="s">
+      <c r="D33" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K33" s="50" t="s">
+      <c r="K33" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="50"/>
-      <c r="U33" s="51"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="53" t="s">
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="34"/>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="136.19999999999999" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="29">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B34" s="30" t="s">
         <v>34</v>
@@ -5064,10 +4329,10 @@
         <v>38</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="33"/>
@@ -5094,38 +4359,32 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="29">
-        <v>147</v>
+        <v>84</v>
       </c>
       <c r="B35" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>191</v>
+        <v>65</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="F35" s="32">
-        <v>45690</v>
-      </c>
-      <c r="G35" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H35" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="I35" s="33" t="s">
-        <v>195</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
       <c r="J35" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K35" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L35" s="34"/>
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
@@ -5138,136 +4397,148 @@
       <c r="U35" s="35"/>
       <c r="V35" s="36"/>
       <c r="W35" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="29">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="B36" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>196</v>
+        <v>67</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="F36" s="32">
-        <v>45691</v>
+        <v>45622</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="J36" s="34" t="s">
         <v>51</v>
       </c>
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
+      <c r="M36" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="O36" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="P36" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q36" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R36" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S36" s="34" t="s">
+        <v>172</v>
+      </c>
       <c r="T36" s="34"/>
       <c r="U36" s="35"/>
       <c r="V36" s="36"/>
       <c r="W36" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="29">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B37" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>201</v>
+        <v>68</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="F37" s="32">
-        <v>45691</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="H37" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="I37" s="33" t="s">
-        <v>205</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F37" s="32"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
       <c r="J37" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K37" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L37" s="34"/>
       <c r="M37" s="34"/>
       <c r="N37" s="34"/>
       <c r="O37" s="34"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="34"/>
-      <c r="S37" s="34"/>
+      <c r="P37" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q37" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R37" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="S37" s="34" t="s">
+        <v>173</v>
+      </c>
       <c r="T37" s="34"/>
       <c r="U37" s="35"/>
       <c r="V37" s="36"/>
       <c r="W37" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="29">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="B38" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>206</v>
+        <v>69</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="F38" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G38" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="H38" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="I38" s="33" t="s">
-        <v>210</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
       <c r="J38" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K38" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L38" s="34" t="s">
+        <v>174</v>
+      </c>
       <c r="M38" s="34"/>
       <c r="N38" s="34"/>
       <c r="O38" s="34"/>
@@ -5279,63 +4550,45 @@
       <c r="U38" s="35"/>
       <c r="V38" s="36"/>
       <c r="W38" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="29">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="B39" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>211</v>
+        <v>70</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="F39" s="32">
-        <v>45660</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="H39" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="I39" s="33" t="s">
-        <v>215</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
       <c r="J39" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N39" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O39" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="P39" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="R39" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S39" s="34" t="s">
-        <v>217</v>
-      </c>
+      <c r="K39" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L39" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
       <c r="T39" s="34"/>
       <c r="U39" s="35"/>
       <c r="V39" s="36"/>
@@ -5343,60 +4596,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="29">
-        <v>152</v>
+        <v>89</v>
       </c>
       <c r="B40" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>218</v>
+        <v>71</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="F40" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="H40" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="I40" s="33" t="s">
-        <v>278</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
       <c r="J40" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N40" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O40" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="P40" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="R40" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S40" s="34" t="s">
-        <v>220</v>
-      </c>
+      <c r="K40" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L40" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34"/>
       <c r="T40" s="34"/>
       <c r="U40" s="35"/>
       <c r="V40" s="36"/>
@@ -5404,21 +4639,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="29">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="B41" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>221</v>
+        <v>73</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="F41" s="32"/>
       <c r="G41" s="33"/>
@@ -5427,9 +4662,11 @@
       <c r="J41" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K41" s="34"/>
+      <c r="K41" s="34" t="s">
+        <v>112</v>
+      </c>
       <c r="L41" s="34" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
       <c r="M41" s="34"/>
       <c r="N41" s="34"/>
@@ -5445,60 +4682,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="29">
-        <v>154</v>
+        <v>91</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>223</v>
+        <v>75</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="F42" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G42" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="H42" s="33" t="s">
-        <v>282</v>
-      </c>
-      <c r="I42" s="33" t="s">
-        <v>284</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
       <c r="J42" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K42" s="34"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N42" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O42" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="P42" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="R42" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S42" s="34" t="s">
-        <v>226</v>
-      </c>
+      <c r="K42" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L42" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="34"/>
       <c r="T42" s="34"/>
       <c r="U42" s="35"/>
       <c r="V42" s="36"/>
@@ -5506,60 +4725,40 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="29">
-        <v>155</v>
+        <v>92</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>227</v>
+        <v>76</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="F43" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G43" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="H43" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="I43" s="33" t="s">
-        <v>229</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
       <c r="J43" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K43" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="K43" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="L43" s="34"/>
-      <c r="M43" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N43" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O43" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="P43" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R43" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S43" s="34" t="s">
-        <v>226</v>
-      </c>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
+      <c r="P43" s="34"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="34"/>
+      <c r="S43" s="34"/>
       <c r="T43" s="34"/>
       <c r="U43" s="35"/>
       <c r="V43" s="36"/>
@@ -5567,21 +4766,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="29">
-        <v>156</v>
+        <v>93</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>231</v>
+        <v>78</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>232</v>
+        <v>140</v>
       </c>
       <c r="F44" s="32"/>
       <c r="G44" s="33"/>
@@ -5608,871 +4807,391 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="29">
-        <v>157</v>
-      </c>
-      <c r="B45" s="30" t="s">
+    <row r="45" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="45"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="50"/>
+      <c r="S45" s="50"/>
+      <c r="T45" s="50"/>
+      <c r="U45" s="51"/>
+      <c r="V45" s="52"/>
+      <c r="W45" s="53"/>
+    </row>
+    <row r="46" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="45"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
+      <c r="S46" s="50"/>
+      <c r="T46" s="50"/>
+      <c r="U46" s="51"/>
+      <c r="V46" s="52"/>
+      <c r="W46" s="53"/>
+    </row>
+    <row r="47" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="54">
+        <v>446</v>
+      </c>
+      <c r="B47" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="F45" s="32"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K45" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L45" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="M45" s="34"/>
-      <c r="N45" s="34"/>
-      <c r="O45" s="34"/>
-      <c r="P45" s="34"/>
-      <c r="Q45" s="34"/>
-      <c r="R45" s="34"/>
-      <c r="S45" s="34"/>
-      <c r="T45" s="34"/>
-      <c r="U45" s="35"/>
-      <c r="V45" s="36"/>
-      <c r="W45" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="29">
-        <v>158</v>
-      </c>
-      <c r="B46" s="30" t="s">
+      <c r="C47" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="F47" s="41">
+        <v>45685</v>
+      </c>
+      <c r="G47" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="H47" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="I47" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="J47" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="43"/>
+      <c r="P47" s="43"/>
+      <c r="Q47" s="43"/>
+      <c r="R47" s="43"/>
+      <c r="S47" s="43"/>
+      <c r="T47" s="43"/>
+      <c r="U47" s="44"/>
+      <c r="V47" s="56"/>
+      <c r="W47" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="162.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="45">
+        <v>447</v>
+      </c>
+      <c r="B48" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="F46" s="32"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K46" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="34"/>
-      <c r="P46" s="34"/>
-      <c r="Q46" s="34"/>
-      <c r="R46" s="34"/>
-      <c r="S46" s="34"/>
-      <c r="T46" s="34"/>
-      <c r="U46" s="35"/>
-      <c r="V46" s="36"/>
-      <c r="W46" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="29">
-        <v>159</v>
-      </c>
-      <c r="B47" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="F47" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G47" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="H47" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="I47" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="J47" s="34" t="s">
+      <c r="C48" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="48">
+        <v>45685</v>
+      </c>
+      <c r="G48" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="H48" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="I48" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="J48" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N47" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O47" s="34" t="s">
-        <v>285</v>
-      </c>
-      <c r="P47" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q47" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="R47" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S47" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="T47" s="34"/>
-      <c r="U47" s="35"/>
-      <c r="V47" s="36"/>
-      <c r="W47" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="29">
-        <v>160</v>
-      </c>
-      <c r="B48" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="F48" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G48" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="H48" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="I48" s="33" t="s">
-        <v>288</v>
-      </c>
-      <c r="J48" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N48" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O48" s="34" t="s">
-        <v>289</v>
-      </c>
-      <c r="P48" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q48" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R48" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S48" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="T48" s="34"/>
-      <c r="U48" s="35"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="29">
-        <v>161</v>
-      </c>
-      <c r="B49" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D49" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="F49" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>291</v>
-      </c>
-      <c r="H49" s="33" t="s">
-        <v>292</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>293</v>
-      </c>
-      <c r="J49" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N49" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O49" s="34" t="s">
-        <v>247</v>
-      </c>
-      <c r="P49" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q49" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R49" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S49" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="T49" s="34"/>
-      <c r="U49" s="35"/>
-      <c r="V49" s="36"/>
-      <c r="W49" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="29">
-        <v>162</v>
-      </c>
-      <c r="B50" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="F50" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G50" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="H50" s="33" t="s">
-        <v>295</v>
-      </c>
-      <c r="I50" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="J50" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
-      <c r="M50" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N50" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O50" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="P50" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q50" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R50" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S50" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="T50" s="34"/>
-      <c r="U50" s="35"/>
-      <c r="V50" s="36"/>
-      <c r="W50" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="29">
-        <v>163</v>
-      </c>
-      <c r="B51" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="F51" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G51" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="H51" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="I51" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="J51" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N51" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O51" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="P51" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q51" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R51" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S51" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="T51" s="34"/>
-      <c r="U51" s="35"/>
-      <c r="V51" s="36"/>
-      <c r="W51" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="29">
-        <v>164</v>
-      </c>
-      <c r="B52" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="E52" s="31" t="s">
-        <v>257</v>
-      </c>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
-      <c r="J52" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K52" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L52" s="34" t="s">
-        <v>258</v>
-      </c>
-      <c r="M52" s="34"/>
-      <c r="N52" s="34"/>
-      <c r="O52" s="34"/>
-      <c r="P52" s="34"/>
-      <c r="Q52" s="34"/>
-      <c r="R52" s="34"/>
-      <c r="S52" s="34"/>
-      <c r="T52" s="34"/>
-      <c r="U52" s="35"/>
-      <c r="V52" s="36"/>
-      <c r="W52" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="29">
-        <v>165</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>259</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="F53" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>301</v>
-      </c>
-      <c r="H53" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="I53" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="J53" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K53" s="34"/>
-      <c r="L53" s="34"/>
-      <c r="M53" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N53" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O53" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="P53" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q53" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R53" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S53" s="34" t="s">
-        <v>264</v>
-      </c>
-      <c r="T53" s="34"/>
-      <c r="U53" s="35"/>
-      <c r="V53" s="36"/>
-      <c r="W53" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="29">
-        <v>166</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="E54" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K54" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="L54" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="34"/>
-      <c r="T54" s="34"/>
-      <c r="U54" s="35"/>
-      <c r="V54" s="36"/>
-      <c r="W54" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="29">
-        <v>167</v>
-      </c>
-      <c r="B55" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="F55" s="32">
-        <v>45692</v>
-      </c>
-      <c r="G55" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="H55" s="33" t="s">
-        <v>304</v>
-      </c>
-      <c r="I55" s="33" t="s">
-        <v>305</v>
-      </c>
-      <c r="J55" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N55" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O55" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="P55" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q55" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R55" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S55" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="T55" s="34"/>
-      <c r="U55" s="35"/>
-      <c r="V55" s="36"/>
-      <c r="W55" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="29">
-        <v>168</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="F56" s="32">
-        <v>45700</v>
-      </c>
-      <c r="G56" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="H56" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="I56" s="33" t="s">
-        <v>319</v>
-      </c>
-      <c r="J56" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N56" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O56" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="P56" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q56" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R56" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S56" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="T56" s="34"/>
-      <c r="U56" s="35"/>
-      <c r="V56" s="36"/>
-      <c r="W56" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" ht="136.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="29">
-        <v>169</v>
-      </c>
-      <c r="B57" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="F57" s="32">
-        <v>45700</v>
-      </c>
-      <c r="G57" s="33" t="s">
-        <v>321</v>
-      </c>
-      <c r="H57" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="I57" s="33" t="s">
-        <v>319</v>
-      </c>
-      <c r="J57" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K57" s="34"/>
-      <c r="L57" s="34"/>
-      <c r="M57" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N57" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O57" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="P57" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q57" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R57" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="S57" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="T57" s="34"/>
-      <c r="U57" s="35"/>
-      <c r="V57" s="36"/>
-      <c r="W57" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="29">
-        <v>374</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="30" t="s">
-        <v>274</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>275</v>
-      </c>
-      <c r="F58" s="32">
-        <v>45700</v>
-      </c>
-      <c r="G58" s="33" t="s">
-        <v>322</v>
-      </c>
-      <c r="H58" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="I58" s="33" t="s">
-        <v>324</v>
-      </c>
-      <c r="J58" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K58" s="34"/>
-      <c r="L58" s="34"/>
-      <c r="M58" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="N58" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="O58" s="34"/>
-      <c r="P58" s="34"/>
-      <c r="Q58" s="34"/>
-      <c r="R58" s="34"/>
-      <c r="S58" s="34"/>
-      <c r="T58" s="34"/>
-      <c r="U58" s="35"/>
-      <c r="V58" s="36"/>
-      <c r="W58" s="37" t="s">
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="50"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="50"/>
+      <c r="R48" s="50"/>
+      <c r="S48" s="50"/>
+      <c r="T48" s="50"/>
+      <c r="U48" s="51"/>
+      <c r="V48" s="52"/>
+      <c r="W48" s="53" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="136.19999999999999" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="29">
-        <v>446</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E59" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="F59" s="32">
-        <v>45685</v>
-      </c>
-      <c r="G59" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H59" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="I59" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="J59" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K59" s="34"/>
-      <c r="L59" s="34"/>
-      <c r="M59" s="34"/>
-      <c r="N59" s="34"/>
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
-      <c r="Q59" s="34"/>
-      <c r="R59" s="34"/>
-      <c r="S59" s="34"/>
-      <c r="T59" s="34"/>
-      <c r="U59" s="35"/>
-      <c r="V59" s="36"/>
-      <c r="W59" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" ht="136.19999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="29">
-        <v>447</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E60" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F60" s="32">
-        <v>45685</v>
-      </c>
-      <c r="G60" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="H60" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="I60" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="J60" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="K60" s="34"/>
-      <c r="L60" s="34"/>
-      <c r="M60" s="34"/>
-      <c r="N60" s="34"/>
-      <c r="O60" s="34"/>
-      <c r="P60" s="34"/>
-      <c r="Q60" s="34"/>
-      <c r="R60" s="34"/>
-      <c r="S60" s="34"/>
-      <c r="T60" s="34"/>
-      <c r="U60" s="35"/>
-      <c r="V60" s="36"/>
-      <c r="W60" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="9"/>
+    </row>
+    <row r="50" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="9"/>
+    </row>
+    <row r="51" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="9"/>
+    </row>
+    <row r="52" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="9"/>
+    </row>
+    <row r="53" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="9"/>
+    </row>
+    <row r="54" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="9"/>
+    </row>
+    <row r="55" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="9"/>
+    </row>
+    <row r="56" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="9"/>
+    </row>
+    <row r="57" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="8"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="9"/>
+    </row>
+    <row r="58" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="9"/>
+    </row>
+    <row r="59" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+      <c r="U59" s="8"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="9"/>
+    </row>
+    <row r="60" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="8"/>
+      <c r="V60" s="2"/>
+      <c r="W60" s="9"/>
+    </row>
+    <row r="61" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
@@ -6492,7 +5211,7 @@
       <c r="V61" s="2"/>
       <c r="W61" s="9"/>
     </row>
-    <row r="62" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
@@ -6512,7 +5231,7 @@
       <c r="V62" s="2"/>
       <c r="W62" s="9"/>
     </row>
-    <row r="63" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
@@ -6532,7 +5251,7 @@
       <c r="V63" s="2"/>
       <c r="W63" s="9"/>
     </row>
-    <row r="64" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
@@ -9333,66 +8052,270 @@
       <c r="W203" s="9"/>
     </row>
     <row r="204" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W204" s="7"/>
+      <c r="F204" s="6"/>
+      <c r="G204" s="6"/>
+      <c r="H204" s="6"/>
+      <c r="I204" s="6"/>
+      <c r="J204" s="7"/>
+      <c r="K204" s="7"/>
+      <c r="L204" s="7"/>
+      <c r="M204" s="7"/>
+      <c r="N204" s="7"/>
+      <c r="O204" s="7"/>
+      <c r="P204" s="7"/>
+      <c r="Q204" s="7"/>
+      <c r="R204" s="7"/>
+      <c r="S204" s="7"/>
+      <c r="T204" s="7"/>
+      <c r="U204" s="8"/>
+      <c r="V204" s="2"/>
+      <c r="W204" s="9"/>
     </row>
     <row r="205" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W205" s="7"/>
+      <c r="F205" s="6"/>
+      <c r="G205" s="6"/>
+      <c r="H205" s="6"/>
+      <c r="I205" s="6"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="M205" s="7"/>
+      <c r="N205" s="7"/>
+      <c r="O205" s="7"/>
+      <c r="P205" s="7"/>
+      <c r="Q205" s="7"/>
+      <c r="R205" s="7"/>
+      <c r="S205" s="7"/>
+      <c r="T205" s="7"/>
+      <c r="U205" s="8"/>
+      <c r="V205" s="2"/>
+      <c r="W205" s="9"/>
     </row>
     <row r="206" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W206" s="7"/>
+      <c r="F206" s="6"/>
+      <c r="G206" s="6"/>
+      <c r="H206" s="6"/>
+      <c r="I206" s="6"/>
+      <c r="J206" s="7"/>
+      <c r="K206" s="7"/>
+      <c r="L206" s="7"/>
+      <c r="M206" s="7"/>
+      <c r="N206" s="7"/>
+      <c r="O206" s="7"/>
+      <c r="P206" s="7"/>
+      <c r="Q206" s="7"/>
+      <c r="R206" s="7"/>
+      <c r="S206" s="7"/>
+      <c r="T206" s="7"/>
+      <c r="U206" s="8"/>
+      <c r="V206" s="2"/>
+      <c r="W206" s="9"/>
     </row>
     <row r="207" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W207" s="7"/>
+      <c r="F207" s="6"/>
+      <c r="G207" s="6"/>
+      <c r="H207" s="6"/>
+      <c r="I207" s="6"/>
+      <c r="J207" s="7"/>
+      <c r="K207" s="7"/>
+      <c r="L207" s="7"/>
+      <c r="M207" s="7"/>
+      <c r="N207" s="7"/>
+      <c r="O207" s="7"/>
+      <c r="P207" s="7"/>
+      <c r="Q207" s="7"/>
+      <c r="R207" s="7"/>
+      <c r="S207" s="7"/>
+      <c r="T207" s="7"/>
+      <c r="U207" s="8"/>
+      <c r="V207" s="2"/>
+      <c r="W207" s="9"/>
     </row>
     <row r="208" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W208" s="7"/>
-    </row>
-    <row r="209" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W209" s="7"/>
-    </row>
-    <row r="210" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W210" s="7"/>
-    </row>
-    <row r="211" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W211" s="7"/>
-    </row>
-    <row r="212" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W212" s="7"/>
-    </row>
-    <row r="213" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W213" s="7"/>
-    </row>
-    <row r="214" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W214" s="7"/>
-    </row>
-    <row r="215" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="W215" s="7"/>
-    </row>
-    <row r="216" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F208" s="6"/>
+      <c r="G208" s="6"/>
+      <c r="H208" s="6"/>
+      <c r="I208" s="6"/>
+      <c r="J208" s="7"/>
+      <c r="K208" s="7"/>
+      <c r="L208" s="7"/>
+      <c r="M208" s="7"/>
+      <c r="N208" s="7"/>
+      <c r="O208" s="7"/>
+      <c r="P208" s="7"/>
+      <c r="Q208" s="7"/>
+      <c r="R208" s="7"/>
+      <c r="S208" s="7"/>
+      <c r="T208" s="7"/>
+      <c r="U208" s="8"/>
+      <c r="V208" s="2"/>
+      <c r="W208" s="9"/>
+    </row>
+    <row r="209" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F209" s="6"/>
+      <c r="G209" s="6"/>
+      <c r="H209" s="6"/>
+      <c r="I209" s="6"/>
+      <c r="J209" s="7"/>
+      <c r="K209" s="7"/>
+      <c r="L209" s="7"/>
+      <c r="M209" s="7"/>
+      <c r="N209" s="7"/>
+      <c r="O209" s="7"/>
+      <c r="P209" s="7"/>
+      <c r="Q209" s="7"/>
+      <c r="R209" s="7"/>
+      <c r="S209" s="7"/>
+      <c r="T209" s="7"/>
+      <c r="U209" s="8"/>
+      <c r="V209" s="2"/>
+      <c r="W209" s="9"/>
+    </row>
+    <row r="210" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F210" s="6"/>
+      <c r="G210" s="6"/>
+      <c r="H210" s="6"/>
+      <c r="I210" s="6"/>
+      <c r="J210" s="7"/>
+      <c r="K210" s="7"/>
+      <c r="L210" s="7"/>
+      <c r="M210" s="7"/>
+      <c r="N210" s="7"/>
+      <c r="O210" s="7"/>
+      <c r="P210" s="7"/>
+      <c r="Q210" s="7"/>
+      <c r="R210" s="7"/>
+      <c r="S210" s="7"/>
+      <c r="T210" s="7"/>
+      <c r="U210" s="8"/>
+      <c r="V210" s="2"/>
+      <c r="W210" s="9"/>
+    </row>
+    <row r="211" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F211" s="6"/>
+      <c r="G211" s="6"/>
+      <c r="H211" s="6"/>
+      <c r="I211" s="6"/>
+      <c r="J211" s="7"/>
+      <c r="K211" s="7"/>
+      <c r="L211" s="7"/>
+      <c r="M211" s="7"/>
+      <c r="N211" s="7"/>
+      <c r="O211" s="7"/>
+      <c r="P211" s="7"/>
+      <c r="Q211" s="7"/>
+      <c r="R211" s="7"/>
+      <c r="S211" s="7"/>
+      <c r="T211" s="7"/>
+      <c r="U211" s="8"/>
+      <c r="V211" s="2"/>
+      <c r="W211" s="9"/>
+    </row>
+    <row r="212" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F212" s="6"/>
+      <c r="G212" s="6"/>
+      <c r="H212" s="6"/>
+      <c r="I212" s="6"/>
+      <c r="J212" s="7"/>
+      <c r="K212" s="7"/>
+      <c r="L212" s="7"/>
+      <c r="M212" s="7"/>
+      <c r="N212" s="7"/>
+      <c r="O212" s="7"/>
+      <c r="P212" s="7"/>
+      <c r="Q212" s="7"/>
+      <c r="R212" s="7"/>
+      <c r="S212" s="7"/>
+      <c r="T212" s="7"/>
+      <c r="U212" s="8"/>
+      <c r="V212" s="2"/>
+      <c r="W212" s="9"/>
+    </row>
+    <row r="213" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F213" s="6"/>
+      <c r="G213" s="6"/>
+      <c r="H213" s="6"/>
+      <c r="I213" s="6"/>
+      <c r="J213" s="7"/>
+      <c r="K213" s="7"/>
+      <c r="L213" s="7"/>
+      <c r="M213" s="7"/>
+      <c r="N213" s="7"/>
+      <c r="O213" s="7"/>
+      <c r="P213" s="7"/>
+      <c r="Q213" s="7"/>
+      <c r="R213" s="7"/>
+      <c r="S213" s="7"/>
+      <c r="T213" s="7"/>
+      <c r="U213" s="8"/>
+      <c r="V213" s="2"/>
+      <c r="W213" s="9"/>
+    </row>
+    <row r="214" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F214" s="6"/>
+      <c r="G214" s="6"/>
+      <c r="H214" s="6"/>
+      <c r="I214" s="6"/>
+      <c r="J214" s="7"/>
+      <c r="K214" s="7"/>
+      <c r="L214" s="7"/>
+      <c r="M214" s="7"/>
+      <c r="N214" s="7"/>
+      <c r="O214" s="7"/>
+      <c r="P214" s="7"/>
+      <c r="Q214" s="7"/>
+      <c r="R214" s="7"/>
+      <c r="S214" s="7"/>
+      <c r="T214" s="7"/>
+      <c r="U214" s="8"/>
+      <c r="V214" s="2"/>
+      <c r="W214" s="9"/>
+    </row>
+    <row r="215" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F215" s="6"/>
+      <c r="G215" s="6"/>
+      <c r="H215" s="6"/>
+      <c r="I215" s="6"/>
+      <c r="J215" s="7"/>
+      <c r="K215" s="7"/>
+      <c r="L215" s="7"/>
+      <c r="M215" s="7"/>
+      <c r="N215" s="7"/>
+      <c r="O215" s="7"/>
+      <c r="P215" s="7"/>
+      <c r="Q215" s="7"/>
+      <c r="R215" s="7"/>
+      <c r="S215" s="7"/>
+      <c r="T215" s="7"/>
+      <c r="U215" s="8"/>
+      <c r="V215" s="2"/>
+      <c r="W215" s="9"/>
+    </row>
+    <row r="216" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W216" s="7"/>
     </row>
-    <row r="217" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W217" s="7"/>
     </row>
-    <row r="218" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W218" s="7"/>
     </row>
-    <row r="219" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W219" s="7"/>
     </row>
-    <row r="220" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W220" s="7"/>
     </row>
-    <row r="221" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W221" s="7"/>
     </row>
-    <row r="222" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W222" s="7"/>
     </row>
-    <row r="223" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W223" s="7"/>
     </row>
-    <row r="224" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W224" s="7"/>
     </row>
     <row r="225" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -10583,16 +9506,49 @@
     <row r="620" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W620" s="7"/>
     </row>
+    <row r="621" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W621" s="7"/>
+    </row>
+    <row r="622" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W622" s="7"/>
+    </row>
+    <row r="623" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W623" s="7"/>
+    </row>
+    <row r="624" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W624" s="7"/>
+    </row>
+    <row r="625" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W625" s="7"/>
+    </row>
+    <row r="626" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W626" s="7"/>
+    </row>
+    <row r="627" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W627" s="7"/>
+    </row>
+    <row r="628" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W628" s="7"/>
+    </row>
+    <row r="629" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W629" s="7"/>
+    </row>
+    <row r="630" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W630" s="7"/>
+    </row>
+    <row r="631" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W631" s="7"/>
+    </row>
+    <row r="632" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W632" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:W60" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <autoFilter ref="A9:W48" xr:uid="{00000000-0001-0000-0200-000000000000}">
     <filterColumn colId="2">
-      <filters>
-        <filter val="RSA"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:W60">
-      <sortCondition ref="A9:A60"/>
-    </sortState>
   </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
@@ -10605,8 +9561,8 @@
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -10614,19 +9570,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M10:N33 P10:R33 J10:J33</xm:sqref>
+          <xm:sqref>P10:R48 J10:J48 M10:N48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T10:T33</xm:sqref>
+          <xm:sqref>T10:T48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K33</xm:sqref>
+          <xm:sqref>K10:K48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10695,7 +9651,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10729,7 +9685,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -10743,7 +9699,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>37</v>
       </c>
@@ -10757,7 +9713,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
@@ -10771,7 +9727,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
@@ -10785,7 +9741,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -10799,7 +9755,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -10813,7 +9769,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -10827,7 +9783,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -10841,7 +9797,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>96</v>
       </c>
@@ -10855,7 +9811,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>121</v>
       </c>
@@ -12873,6 +11829,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13130,42 +12107,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13188,9 +12133,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix error mancato accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33991313-E2F5-4F99-B344-6728EFC8640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4328AFF0-7354-4C4E-B339-860BD1D531D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,9 +961,6 @@
     <t>[ERRORE-b36| Sezione Storia Clinica: l'elemento entry/organizer/subject/relatedSubject deve avere l'attributo @classCode='PRS' e deve contenere l'elemento 'code'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Nota di consulto'--&gt; ]</t>
   </si>
   <si>
-    <t>Gestito dall'aplicaizone</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
   </si>
   <si>
@@ -1216,15 +1213,6 @@
     <t>14fac2c7eff93ce5</t>
   </si>
   <si>
-    <t>2025-03-11T11:20:17Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.f5948120a53fd0f82225c83623d436c850de264c43f62cab45c56573de35d2fe.a6acf65a39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7378963bcae8c7da</t>
-  </si>
-  <si>
     <t>2025-03-11T11:29:49Z</t>
   </si>
   <si>
@@ -1259,6 +1247,18 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.b5c4d2747efa33e4350dbbdfd24ac6a850a68364da5120e6086f5520d637e195.ddd1062b7a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-03-11T16:26:23Z</t>
+  </si>
+  <si>
+    <t>807ba7db3098f1be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.f5948120a53fd0f82225c83623d436c850de264c43f62cab45c56573de35d2fe.3fe8320dbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>L'errore viene gestito dall'aplicaizone, controllando che sia stato inserito il valore. Nel caso risultasse vuoto viene mostrato un messaggio di errore</t>
   </si>
 </sst>
 </file>
@@ -3536,10 +3536,10 @@
   <dimension ref="A1:W620"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H53" sqref="H53"/>
+      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3844,7 +3844,7 @@
         <v>45714</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H10" s="33" t="s">
         <v>161</v>
@@ -3898,7 +3898,7 @@
         <v>48</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>44</v>
@@ -3907,10 +3907,10 @@
         <v>45727</v>
       </c>
       <c r="G11" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>308</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>309</v>
       </c>
       <c r="I11" s="33" t="s">
         <v>141</v>
@@ -3939,7 +3939,7 @@
         <v>51</v>
       </c>
       <c r="S11" s="34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T11" s="34"/>
       <c r="U11" s="35"/>
@@ -3968,7 +3968,7 @@
         <v>45714</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H12" s="33" t="s">
         <v>162</v>
@@ -4022,7 +4022,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>49</v>
@@ -4031,10 +4031,10 @@
         <v>45727</v>
       </c>
       <c r="G13" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="H13" s="33" t="s">
         <v>301</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>302</v>
       </c>
       <c r="I13" s="33" t="s">
         <v>141</v>
@@ -4051,7 +4051,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P13" s="34" t="s">
         <v>51</v>
@@ -4063,7 +4063,7 @@
         <v>101</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T13" s="34"/>
       <c r="U13" s="35"/>
@@ -4140,7 +4140,7 @@
         <v>48</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>113</v>
@@ -4165,7 +4165,7 @@
         <v>51</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P15" s="34" t="s">
         <v>51</v>
@@ -4177,7 +4177,7 @@
         <v>101</v>
       </c>
       <c r="S15" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T15" s="34"/>
       <c r="U15" s="35" t="s">
@@ -4208,10 +4208,10 @@
         <v>45714</v>
       </c>
       <c r="G16" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="H16" s="33" t="s">
         <v>282</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>283</v>
       </c>
       <c r="I16" s="33" t="s">
         <v>148</v>
@@ -4228,7 +4228,7 @@
         <v>51</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P16" s="34" t="s">
         <v>51</v>
@@ -4271,13 +4271,13 @@
         <v>45714</v>
       </c>
       <c r="G17" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="H17" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="I17" s="33" t="s">
         <v>286</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>287</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>51</v>
@@ -4291,7 +4291,7 @@
         <v>51</v>
       </c>
       <c r="O17" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P17" s="34" t="s">
         <v>51</v>
@@ -4375,13 +4375,13 @@
         <v>45714</v>
       </c>
       <c r="G19" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="H19" s="33" t="s">
         <v>289</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="I19" s="33" t="s">
         <v>290</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>291</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>51</v>
@@ -4395,7 +4395,7 @@
         <v>51</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P19" s="34" t="s">
         <v>51</v>
@@ -4436,13 +4436,13 @@
         <v>45727</v>
       </c>
       <c r="G20" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="H20" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="I20" s="33" t="s">
         <v>305</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>306</v>
       </c>
       <c r="J20" s="34" t="s">
         <v>51</v>
@@ -4468,7 +4468,7 @@
         <v>51</v>
       </c>
       <c r="S20" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="T20" s="34"/>
       <c r="U20" s="35"/>
@@ -4702,13 +4702,13 @@
         <v>45987</v>
       </c>
       <c r="G26" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>293</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="I26" s="33" t="s">
         <v>294</v>
-      </c>
-      <c r="I26" s="33" t="s">
-        <v>295</v>
       </c>
       <c r="J26" s="34" t="s">
         <v>51</v>
@@ -4722,7 +4722,7 @@
         <v>51</v>
       </c>
       <c r="O26" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P26" s="34" t="s">
         <v>51</v>
@@ -4991,7 +4991,7 @@
         <v>112</v>
       </c>
       <c r="L32" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M32" s="43"/>
       <c r="N32" s="43"/>
@@ -5109,13 +5109,13 @@
         <v>45727</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H35" s="33" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I35" s="33" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>51</v>
@@ -5297,13 +5297,13 @@
         <v>45727</v>
       </c>
       <c r="G39" s="33" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>51</v>
@@ -5358,13 +5358,13 @@
         <v>45692</v>
       </c>
       <c r="G40" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H40" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="I40" s="33" t="s">
         <v>240</v>
-      </c>
-      <c r="I40" s="33" t="s">
-        <v>241</v>
       </c>
       <c r="J40" s="34" t="s">
         <v>51</v>
@@ -5378,7 +5378,7 @@
         <v>51</v>
       </c>
       <c r="O40" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P40" s="34" t="s">
         <v>51</v>
@@ -5460,13 +5460,13 @@
         <v>45692</v>
       </c>
       <c r="G42" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="H42" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="I42" s="33" t="s">
         <v>244</v>
-      </c>
-      <c r="H42" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="33" t="s">
-        <v>245</v>
       </c>
       <c r="J42" s="34" t="s">
         <v>51</v>
@@ -5521,13 +5521,13 @@
         <v>45727</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="H43" s="33" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="J43" s="34" t="s">
         <v>51</v>
@@ -5707,10 +5707,10 @@
         <v>45692</v>
       </c>
       <c r="G47" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="H47" s="33" t="s">
         <v>247</v>
-      </c>
-      <c r="H47" s="33" t="s">
-        <v>248</v>
       </c>
       <c r="I47" s="33" t="s">
         <v>204</v>
@@ -5727,7 +5727,7 @@
         <v>51</v>
       </c>
       <c r="O47" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P47" s="34" t="s">
         <v>51</v>
@@ -5768,13 +5768,13 @@
         <v>45692</v>
       </c>
       <c r="G48" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>208</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J48" s="34" t="s">
         <v>51</v>
@@ -5788,7 +5788,7 @@
         <v>51</v>
       </c>
       <c r="O48" s="34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P48" s="34" t="s">
         <v>51</v>
@@ -5829,13 +5829,13 @@
         <v>45692</v>
       </c>
       <c r="G49" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="H49" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="H49" s="33" t="s">
+      <c r="I49" s="33" t="s">
         <v>253</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>254</v>
       </c>
       <c r="J49" s="34" t="s">
         <v>51</v>
@@ -5890,13 +5890,13 @@
         <v>45692</v>
       </c>
       <c r="G50" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="H50" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="H50" s="33" t="s">
+      <c r="I50" s="33" t="s">
         <v>256</v>
-      </c>
-      <c r="I50" s="33" t="s">
-        <v>257</v>
       </c>
       <c r="J50" s="34" t="s">
         <v>51</v>
@@ -5951,13 +5951,13 @@
         <v>45692</v>
       </c>
       <c r="G51" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="H51" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="H51" s="33" t="s">
+      <c r="I51" s="33" t="s">
         <v>260</v>
-      </c>
-      <c r="I51" s="33" t="s">
-        <v>261</v>
       </c>
       <c r="J51" s="34" t="s">
         <v>51</v>
@@ -5971,7 +5971,7 @@
         <v>51</v>
       </c>
       <c r="O51" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P51" s="34" t="s">
         <v>51</v>
@@ -6055,13 +6055,13 @@
         <v>45727</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="H53" s="33" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J53" s="34" t="s">
         <v>51</v>
@@ -6087,7 +6087,7 @@
         <v>51</v>
       </c>
       <c r="S53" s="34" t="s">
-        <v>227</v>
+        <v>324</v>
       </c>
       <c r="T53" s="34"/>
       <c r="U53" s="35"/>
@@ -6107,10 +6107,10 @@
         <v>48</v>
       </c>
       <c r="D54" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E54" s="31" t="s">
         <v>228</v>
-      </c>
-      <c r="E54" s="31" t="s">
-        <v>229</v>
       </c>
       <c r="F54" s="32"/>
       <c r="G54" s="33"/>
@@ -6150,22 +6150,22 @@
         <v>48</v>
       </c>
       <c r="D55" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" s="31" t="s">
         <v>230</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>231</v>
       </c>
       <c r="F55" s="32">
         <v>45692</v>
       </c>
       <c r="G55" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="H55" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="H55" s="33" t="s">
+      <c r="I55" s="33" t="s">
         <v>264</v>
-      </c>
-      <c r="I55" s="33" t="s">
-        <v>265</v>
       </c>
       <c r="J55" s="34" t="s">
         <v>51</v>
@@ -6179,7 +6179,7 @@
         <v>51</v>
       </c>
       <c r="O55" s="34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P55" s="34" t="s">
         <v>51</v>
@@ -6191,7 +6191,7 @@
         <v>51</v>
       </c>
       <c r="S55" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T55" s="34"/>
       <c r="U55" s="35"/>
@@ -6211,22 +6211,22 @@
         <v>48</v>
       </c>
       <c r="D56" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E56" s="31" t="s">
         <v>233</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>234</v>
       </c>
       <c r="F56" s="32">
         <v>45700</v>
       </c>
       <c r="G56" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="H56" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="H56" s="33" t="s">
+      <c r="I56" s="33" t="s">
         <v>273</v>
-      </c>
-      <c r="I56" s="33" t="s">
-        <v>274</v>
       </c>
       <c r="J56" s="34" t="s">
         <v>51</v>
@@ -6240,7 +6240,7 @@
         <v>51</v>
       </c>
       <c r="O56" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P56" s="34" t="s">
         <v>51</v>
@@ -6252,7 +6252,7 @@
         <v>51</v>
       </c>
       <c r="S56" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T56" s="34"/>
       <c r="U56" s="35"/>
@@ -6272,22 +6272,22 @@
         <v>48</v>
       </c>
       <c r="D57" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="E57" s="31" t="s">
         <v>235</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>236</v>
       </c>
       <c r="F57" s="32">
         <v>45700</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H57" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="I57" s="33" t="s">
         <v>273</v>
-      </c>
-      <c r="I57" s="33" t="s">
-        <v>274</v>
       </c>
       <c r="J57" s="34" t="s">
         <v>51</v>
@@ -6301,7 +6301,7 @@
         <v>51</v>
       </c>
       <c r="O57" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P57" s="34" t="s">
         <v>51</v>
@@ -6313,7 +6313,7 @@
         <v>51</v>
       </c>
       <c r="S57" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T57" s="34"/>
       <c r="U57" s="35"/>
@@ -6333,22 +6333,22 @@
         <v>48</v>
       </c>
       <c r="D58" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E58" s="31" t="s">
         <v>237</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>238</v>
       </c>
       <c r="F58" s="32">
         <v>45700</v>
       </c>
       <c r="G58" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="H58" s="33" t="s">
         <v>277</v>
       </c>
-      <c r="H58" s="33" t="s">
+      <c r="I58" s="33" t="s">
         <v>278</v>
-      </c>
-      <c r="I58" s="33" t="s">
-        <v>279</v>
       </c>
       <c r="J58" s="34" t="s">
         <v>51</v>
@@ -6393,13 +6393,13 @@
         <v>45714</v>
       </c>
       <c r="G59" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="H59" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="H59" s="33" t="s">
+      <c r="I59" s="33" t="s">
         <v>298</v>
-      </c>
-      <c r="I59" s="33" t="s">
-        <v>299</v>
       </c>
       <c r="J59" s="34" t="s">
         <v>51</v>
@@ -6440,13 +6440,13 @@
         <v>45727</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="I60" s="33" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="J60" s="34" t="s">
         <v>51</v>
@@ -10681,7 +10681,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12859,27 +12859,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13137,10 +13116,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13163,20 +13174,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix error 165 test
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4328AFF0-7354-4C4E-B339-860BD1D531D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE045569-EE16-4997-8A8A-77B9D014D3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1240,15 +1240,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.59f2115922b9a9248be9414eb10c2673ca7f9624d9b2ae1c678103d930c49cbe.6474836e39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-03-11T12:09:04Z</t>
-  </si>
-  <si>
-    <t>3c6a772ec477156c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b5c4d2747efa33e4350dbbdfd24ac6a850a68364da5120e6086f5520d637e195.ddd1062b7a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2025-03-11T16:26:23Z</t>
   </si>
   <si>
@@ -1259,6 +1250,15 @@
   </si>
   <si>
     <t>L'errore viene gestito dall'aplicaizone, controllando che sia stato inserito il valore. Nel caso risultasse vuoto viene mostrato un messaggio di errore</t>
+  </si>
+  <si>
+    <t>2025-03-14T12:29:43Z</t>
+  </si>
+  <si>
+    <t>e03c29ecf006c5a3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b5c4d2747efa33e4350dbbdfd24ac6a850a68364da5120e6086f5520d637e195.b4f004885a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3536,7 +3536,7 @@
   <dimension ref="A1:W620"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
@@ -6052,16 +6052,16 @@
         <v>225</v>
       </c>
       <c r="F53" s="32">
-        <v>45727</v>
+        <v>45730</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="H53" s="33" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="J53" s="34" t="s">
         <v>51</v>
@@ -6087,7 +6087,7 @@
         <v>51</v>
       </c>
       <c r="S53" s="34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="T53" s="34"/>
       <c r="U53" s="35"/>
@@ -6440,13 +6440,13 @@
         <v>45727</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I60" s="33" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J60" s="34" t="s">
         <v>51</v>
@@ -12859,6 +12859,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13116,42 +13137,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13174,9 +13163,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Dettaglio colonna gestione errore.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GENIUSSRLXX/GENIUSRL/POCR/1.0.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Personal\it-fse-accreditamento\GATEWAY\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\A1#111#GENIUSSRLXX\GENIUSRL\POCR\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185241CC-1824-40BA-BB00-99BFD9CAA2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956B600E-C05D-409A-A05A-5D769661E495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,37 +686,16 @@
     <t>Il campo purpose_of_use non è valorizzato</t>
   </si>
   <si>
-    <t>VIENE SEGNALATO UN ERRORE ALL'UTENTE</t>
-  </si>
-  <si>
     <t>Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>Il campo action_id non è corretto, Token non valido</t>
-  </si>
-  <si>
     <t xml:space="preserve">ERRORE DI TIME OUT </t>
   </si>
   <si>
-    <t>ERRORE DI TIME OUT</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.8145520e9ad427cd401945e0791d3026c2f2f35353746df9e199468a3214874f.c01a152e85^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>File xml CDA non valido</t>
-  </si>
-  <si>
-    <t>Codice fiscale cittadino non valido</t>
-  </si>
-  <si>
-    <t>Dati cittadino mancanti</t>
-  </si>
-  <si>
     <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
-  </si>
-  <si>
-    <t>Referto vuoto</t>
   </si>
   <si>
     <t>NON INVIAMO I PRECEDENTI</t>
@@ -1087,9 +1066,6 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>Viene fornito un messaggio di errore all'utente, campi token non validi</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_RSA_TIMEOUT</t>
   </si>
   <si>
@@ -1259,6 +1235,33 @@
   </si>
   <si>
     <t>c7302c1e18ade65a</t>
+  </si>
+  <si>
+    <t>È stato rilevato un errore di connessione al gateway dovuto alla mancata valorizzazione del campo purpose_of_use. Si invita a segnalare il problema all'amministratore di sistema per le opportune verifiche.
+L'operatore dedicato provvederà ad aggiornare il software con i parametri corretti per la generazione dei token JWT, assicurando così l’inclusione del campo purpose_of_use. Successivamente, si procederà alla validazione e all'invio dei referti.</t>
+  </si>
+  <si>
+    <t>È stato riscontrato un errore di connessione al gateway, attribuibile a un'impostazione non corretta del campo action_id. Si raccomanda di informare l'amministratore di sistema affinché possa effettuare le verifiche necessarie.
+L'operatore incaricato provvederà a configurare correttamente i parametri per la generazione del token JWT all'interno del software, includendo il valore corretto di action_id. Una volta completata la modifica, si procederà con la validazione e il reinvio dei referti.</t>
+  </si>
+  <si>
+    <t>È stato segnalato un errore di connessione al gateway, causato da un valore errato del campo action_id. Si richiede di notificare il problema all’amministratore di sistema per consentire le opportune verifiche.
+L’operatore incaricato provvederà a integrare nel software i parametri necessari per la corretta generazione dei token JWT e, una volta effettuata la correzione, procederà con la validazione e il reinvio dei referti.</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di timeout, si invita l'utente a riprovare il flusso applicativo per la produzione del referto.</t>
+  </si>
+  <si>
+    <t>Durante la creazione del referto, avviene la verifica di questo errore. Qualora il controllo non rilevasse l’anomalia, verrà comunque generato un elenco riepilogativo contenente tutti i referti coinvolti.</t>
+  </si>
+  <si>
+    <t>Durante la creazione del referto, avviene la verifica di questo errore.Indicando all'operatore l'anomalia riscontrata, e si inviata l'operatore alla correzzione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa tipologia di errore viene controlla al momento del salvataggio del referto, pertanto l'intervento di correzione avviene prima della generazione del referto. </t>
+  </si>
+  <si>
+    <t>L'errore viene controllato al salvataggio del referto. Invitando l'operatore alla correzzione e alla produzione corretta dello stesso</t>
   </si>
 </sst>
 </file>
@@ -3536,10 +3539,10 @@
   <dimension ref="A1:W620"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H54" sqref="H54"/>
+      <selection pane="bottomRight" activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3612,7 +3615,7 @@
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="69" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D3" s="61"/>
       <c r="F3" s="6"/>
@@ -3638,7 +3641,7 @@
       <c r="A4" s="65"/>
       <c r="B4" s="66"/>
       <c r="C4" s="69" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="4"/>
@@ -3665,7 +3668,7 @@
       <c r="A5" s="67"/>
       <c r="B5" s="68"/>
       <c r="C5" s="69" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D5" s="61"/>
       <c r="F5" s="6"/>
@@ -3844,10 +3847,10 @@
         <v>45714</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I10" s="33" t="s">
         <v>141</v>
@@ -3876,7 +3879,7 @@
         <v>101</v>
       </c>
       <c r="S10" s="34" t="s">
-        <v>143</v>
+        <v>317</v>
       </c>
       <c r="T10" s="34"/>
       <c r="U10" s="35" t="s">
@@ -3898,7 +3901,7 @@
         <v>48</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>44</v>
@@ -3907,10 +3910,10 @@
         <v>45727</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="I11" s="33" t="s">
         <v>141</v>
@@ -3939,7 +3942,7 @@
         <v>51</v>
       </c>
       <c r="S11" s="34" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="T11" s="34"/>
       <c r="U11" s="35"/>
@@ -3968,10 +3971,10 @@
         <v>45714</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I12" s="33" t="s">
         <v>141</v>
@@ -3988,7 +3991,7 @@
         <v>51</v>
       </c>
       <c r="O12" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P12" s="34" t="s">
         <v>51</v>
@@ -4000,7 +4003,7 @@
         <v>101</v>
       </c>
       <c r="S12" s="34" t="s">
-        <v>145</v>
+        <v>318</v>
       </c>
       <c r="T12" s="34"/>
       <c r="U12" s="35" t="s">
@@ -4022,7 +4025,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>49</v>
@@ -4031,10 +4034,10 @@
         <v>45727</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="I13" s="33" t="s">
         <v>141</v>
@@ -4051,7 +4054,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P13" s="34" t="s">
         <v>51</v>
@@ -4063,7 +4066,7 @@
         <v>101</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>267</v>
+        <v>319</v>
       </c>
       <c r="T13" s="34"/>
       <c r="U13" s="35"/>
@@ -4106,7 +4109,7 @@
         <v>51</v>
       </c>
       <c r="O14" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P14" s="34" t="s">
         <v>51</v>
@@ -4118,7 +4121,7 @@
         <v>101</v>
       </c>
       <c r="S14" s="34" t="s">
-        <v>147</v>
+        <v>320</v>
       </c>
       <c r="T14" s="34"/>
       <c r="U14" s="35" t="s">
@@ -4140,7 +4143,7 @@
         <v>48</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>113</v>
@@ -4165,7 +4168,7 @@
         <v>51</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="P15" s="34" t="s">
         <v>51</v>
@@ -4177,7 +4180,7 @@
         <v>101</v>
       </c>
       <c r="S15" s="34" t="s">
-        <v>269</v>
+        <v>320</v>
       </c>
       <c r="T15" s="34"/>
       <c r="U15" s="35" t="s">
@@ -4208,13 +4211,13 @@
         <v>45714</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="I16" s="33" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J16" s="34" t="s">
         <v>51</v>
@@ -4228,7 +4231,7 @@
         <v>51</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="P16" s="34" t="s">
         <v>51</v>
@@ -4240,7 +4243,7 @@
         <v>101</v>
       </c>
       <c r="S16" s="34" t="s">
-        <v>149</v>
+        <v>321</v>
       </c>
       <c r="T16" s="34"/>
       <c r="U16" s="35" t="s">
@@ -4271,13 +4274,13 @@
         <v>45714</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="I17" s="33" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>51</v>
@@ -4291,7 +4294,7 @@
         <v>51</v>
       </c>
       <c r="O17" s="34" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="P17" s="34" t="s">
         <v>51</v>
@@ -4303,7 +4306,7 @@
         <v>101</v>
       </c>
       <c r="S17" s="34" t="s">
-        <v>150</v>
+        <v>322</v>
       </c>
       <c r="T17" s="34"/>
       <c r="U17" s="35" t="s">
@@ -4375,13 +4378,13 @@
         <v>45714</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="I19" s="33" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>51</v>
@@ -4395,7 +4398,7 @@
         <v>51</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="P19" s="34" t="s">
         <v>51</v>
@@ -4407,7 +4410,7 @@
         <v>101</v>
       </c>
       <c r="S19" s="34" t="s">
-        <v>151</v>
+        <v>323</v>
       </c>
       <c r="T19" s="34"/>
       <c r="U19" s="35"/>
@@ -4436,13 +4439,13 @@
         <v>45727</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="J20" s="34" t="s">
         <v>51</v>
@@ -4456,7 +4459,7 @@
         <v>51</v>
       </c>
       <c r="O20" s="34" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P20" s="34" t="s">
         <v>51</v>
@@ -4468,7 +4471,7 @@
         <v>51</v>
       </c>
       <c r="S20" s="34" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="T20" s="34"/>
       <c r="U20" s="35"/>
@@ -4702,13 +4705,13 @@
         <v>45987</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="J26" s="34" t="s">
         <v>51</v>
@@ -4722,7 +4725,7 @@
         <v>51</v>
       </c>
       <c r="O26" s="34" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="P26" s="34" t="s">
         <v>51</v>
@@ -4734,7 +4737,7 @@
         <v>101</v>
       </c>
       <c r="S26" s="34" t="s">
-        <v>153</v>
+        <v>324</v>
       </c>
       <c r="T26" s="34"/>
       <c r="U26" s="35"/>
@@ -4783,7 +4786,7 @@
         <v>101</v>
       </c>
       <c r="S27" s="34" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="T27" s="34"/>
       <c r="U27" s="35"/>
@@ -4819,7 +4822,7 @@
         <v>112</v>
       </c>
       <c r="L28" s="34" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
@@ -4862,7 +4865,7 @@
         <v>112</v>
       </c>
       <c r="L29" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M29" s="34"/>
       <c r="N29" s="34"/>
@@ -4905,7 +4908,7 @@
         <v>112</v>
       </c>
       <c r="L30" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="M30" s="34"/>
       <c r="N30" s="34"/>
@@ -4948,7 +4951,7 @@
         <v>112</v>
       </c>
       <c r="L31" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
@@ -4991,7 +4994,7 @@
         <v>112</v>
       </c>
       <c r="L32" s="43" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="M32" s="43"/>
       <c r="N32" s="43"/>
@@ -5100,22 +5103,22 @@
         <v>48</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F35" s="32">
         <v>45727</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="H35" s="33" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="I35" s="33" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>51</v>
@@ -5147,22 +5150,22 @@
         <v>48</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F36" s="32">
         <v>45691</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="J36" s="34" t="s">
         <v>51</v>
@@ -5194,22 +5197,22 @@
         <v>48</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F37" s="32">
         <v>45691</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>51</v>
@@ -5241,22 +5244,22 @@
         <v>48</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F38" s="32">
         <v>45692</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="J38" s="34" t="s">
         <v>51</v>
@@ -5288,22 +5291,22 @@
         <v>48</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F39" s="32">
         <v>45727</v>
       </c>
       <c r="G39" s="33" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>51</v>
@@ -5317,7 +5320,7 @@
         <v>51</v>
       </c>
       <c r="O39" s="34" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="P39" s="34" t="s">
         <v>51</v>
@@ -5329,7 +5332,7 @@
         <v>101</v>
       </c>
       <c r="S39" s="34" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="T39" s="34"/>
       <c r="U39" s="35"/>
@@ -5349,22 +5352,22 @@
         <v>48</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F40" s="32">
         <v>45692</v>
       </c>
       <c r="G40" s="33" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H40" s="33" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I40" s="33" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J40" s="34" t="s">
         <v>51</v>
@@ -5378,7 +5381,7 @@
         <v>51</v>
       </c>
       <c r="O40" s="34" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="P40" s="34" t="s">
         <v>51</v>
@@ -5390,7 +5393,7 @@
         <v>101</v>
       </c>
       <c r="S40" s="34" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="T40" s="34"/>
       <c r="U40" s="35"/>
@@ -5410,10 +5413,10 @@
         <v>48</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F41" s="32"/>
       <c r="G41" s="33"/>
@@ -5451,22 +5454,22 @@
         <v>48</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F42" s="32">
         <v>45692</v>
       </c>
       <c r="G42" s="33" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H42" s="33" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="I42" s="33" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="J42" s="34" t="s">
         <v>51</v>
@@ -5480,7 +5483,7 @@
         <v>51</v>
       </c>
       <c r="O42" s="34" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="P42" s="34" t="s">
         <v>51</v>
@@ -5492,7 +5495,7 @@
         <v>51</v>
       </c>
       <c r="S42" s="34" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="T42" s="34"/>
       <c r="U42" s="35"/>
@@ -5512,22 +5515,22 @@
         <v>48</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F43" s="32">
         <v>45727</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="H43" s="33" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="J43" s="34" t="s">
         <v>51</v>
@@ -5541,7 +5544,7 @@
         <v>51</v>
       </c>
       <c r="O43" s="34" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="P43" s="34" t="s">
         <v>51</v>
@@ -5553,7 +5556,7 @@
         <v>51</v>
       </c>
       <c r="S43" s="34" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="T43" s="34"/>
       <c r="U43" s="35"/>
@@ -5573,10 +5576,10 @@
         <v>48</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F44" s="32"/>
       <c r="G44" s="33"/>
@@ -5614,10 +5617,10 @@
         <v>48</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F45" s="32"/>
       <c r="G45" s="33"/>
@@ -5630,7 +5633,7 @@
         <v>112</v>
       </c>
       <c r="L45" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M45" s="34"/>
       <c r="N45" s="34"/>
@@ -5657,10 +5660,10 @@
         <v>48</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F46" s="32"/>
       <c r="G46" s="33"/>
@@ -5698,22 +5701,22 @@
         <v>48</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F47" s="32">
         <v>45692</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H47" s="33" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="I47" s="33" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>51</v>
@@ -5727,7 +5730,7 @@
         <v>51</v>
       </c>
       <c r="O47" s="34" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="P47" s="34" t="s">
         <v>51</v>
@@ -5739,7 +5742,7 @@
         <v>51</v>
       </c>
       <c r="S47" s="34" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="T47" s="34"/>
       <c r="U47" s="35"/>
@@ -5759,22 +5762,22 @@
         <v>48</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F48" s="32">
         <v>45692</v>
       </c>
       <c r="G48" s="33" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="H48" s="33" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="J48" s="34" t="s">
         <v>51</v>
@@ -5788,7 +5791,7 @@
         <v>51</v>
       </c>
       <c r="O48" s="34" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="P48" s="34" t="s">
         <v>51</v>
@@ -5800,7 +5803,7 @@
         <v>51</v>
       </c>
       <c r="S48" s="34" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="T48" s="34"/>
       <c r="U48" s="35"/>
@@ -5820,22 +5823,22 @@
         <v>48</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F49" s="32">
         <v>45692</v>
       </c>
       <c r="G49" s="33" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="H49" s="33" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I49" s="33" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J49" s="34" t="s">
         <v>51</v>
@@ -5849,7 +5852,7 @@
         <v>51</v>
       </c>
       <c r="O49" s="34" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="P49" s="34" t="s">
         <v>51</v>
@@ -5861,7 +5864,7 @@
         <v>51</v>
       </c>
       <c r="S49" s="34" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="T49" s="34"/>
       <c r="U49" s="35"/>
@@ -5881,22 +5884,22 @@
         <v>48</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F50" s="32">
         <v>45692</v>
       </c>
       <c r="G50" s="33" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H50" s="33" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I50" s="33" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J50" s="34" t="s">
         <v>51</v>
@@ -5910,7 +5913,7 @@
         <v>51</v>
       </c>
       <c r="O50" s="34" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="P50" s="34" t="s">
         <v>51</v>
@@ -5922,7 +5925,7 @@
         <v>51</v>
       </c>
       <c r="S50" s="34" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="T50" s="34"/>
       <c r="U50" s="35"/>
@@ -5942,22 +5945,22 @@
         <v>48</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F51" s="32">
         <v>45692</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H51" s="33" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="J51" s="34" t="s">
         <v>51</v>
@@ -5971,7 +5974,7 @@
         <v>51</v>
       </c>
       <c r="O51" s="34" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="P51" s="34" t="s">
         <v>51</v>
@@ -5983,7 +5986,7 @@
         <v>51</v>
       </c>
       <c r="S51" s="34" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="T51" s="34"/>
       <c r="U51" s="35"/>
@@ -6003,10 +6006,10 @@
         <v>48</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F52" s="32"/>
       <c r="G52" s="33"/>
@@ -6019,7 +6022,7 @@
         <v>112</v>
       </c>
       <c r="L52" s="34" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="M52" s="34"/>
       <c r="N52" s="34"/>
@@ -6046,22 +6049,22 @@
         <v>48</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F53" s="32">
         <v>45747</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="H53" s="33" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="J53" s="34" t="s">
         <v>51</v>
@@ -6075,7 +6078,7 @@
         <v>51</v>
       </c>
       <c r="O53" s="34" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="P53" s="34" t="s">
         <v>51</v>
@@ -6087,7 +6090,7 @@
         <v>51</v>
       </c>
       <c r="S53" s="34" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="T53" s="34"/>
       <c r="U53" s="35"/>
@@ -6107,10 +6110,10 @@
         <v>48</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F54" s="32"/>
       <c r="G54" s="33"/>
@@ -6123,7 +6126,7 @@
         <v>112</v>
       </c>
       <c r="L54" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M54" s="34"/>
       <c r="N54" s="34"/>
@@ -6150,22 +6153,22 @@
         <v>48</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F55" s="32">
         <v>45692</v>
       </c>
       <c r="G55" s="33" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H55" s="33" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I55" s="33" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="J55" s="34" t="s">
         <v>51</v>
@@ -6179,7 +6182,7 @@
         <v>51</v>
       </c>
       <c r="O55" s="34" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="P55" s="34" t="s">
         <v>51</v>
@@ -6191,7 +6194,7 @@
         <v>51</v>
       </c>
       <c r="S55" s="34" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="T55" s="34"/>
       <c r="U55" s="35"/>
@@ -6211,22 +6214,22 @@
         <v>48</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F56" s="32">
         <v>45700</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="H56" s="33" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="I56" s="33" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J56" s="34" t="s">
         <v>51</v>
@@ -6240,7 +6243,7 @@
         <v>51</v>
       </c>
       <c r="O56" s="34" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="P56" s="34" t="s">
         <v>51</v>
@@ -6252,7 +6255,7 @@
         <v>51</v>
       </c>
       <c r="S56" s="34" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="T56" s="34"/>
       <c r="U56" s="35"/>
@@ -6272,22 +6275,22 @@
         <v>48</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F57" s="32">
         <v>45700</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="H57" s="33" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="I57" s="33" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J57" s="34" t="s">
         <v>51</v>
@@ -6301,7 +6304,7 @@
         <v>51</v>
       </c>
       <c r="O57" s="34" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="P57" s="34" t="s">
         <v>51</v>
@@ -6313,7 +6316,7 @@
         <v>51</v>
       </c>
       <c r="S57" s="34" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="T57" s="34"/>
       <c r="U57" s="35"/>
@@ -6333,22 +6336,22 @@
         <v>48</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F58" s="32">
         <v>45700</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="H58" s="33" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I58" s="33" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J58" s="34" t="s">
         <v>51</v>
@@ -6393,13 +6396,13 @@
         <v>45714</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H59" s="33" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="I59" s="33" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J59" s="34" t="s">
         <v>51</v>
@@ -6440,13 +6443,13 @@
         <v>45727</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I60" s="33" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="J60" s="34" t="s">
         <v>51</v>
@@ -12859,27 +12862,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13137,10 +13119,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13163,20 +13177,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>